<commit_message>
Updated story tracker end of sprint 1
</commit_message>
<xml_diff>
--- a/User Story Tracker.xlsx
+++ b/User Story Tracker.xlsx
@@ -1,27 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SA276\Documents\GitHub\ITTeamProject_Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\ITGroupProject_Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5E127205-19AC-47C1-914C-E18701F21284}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2210F1B9-8FF8-4142-AAB6-AB255B973684}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{12D98D7F-908C-47C5-A977-B7011EB041AE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{12D98D7F-908C-47C5-A977-B7011EB041AE}"/>
   </bookViews>
   <sheets>
     <sheet name="Timeline" sheetId="6" r:id="rId1"/>
     <sheet name="User Stories Sprint 1" sheetId="2" r:id="rId2"/>
     <sheet name="Tasks Sprint 1" sheetId="3" r:id="rId3"/>
     <sheet name="User Stories Sprint 2" sheetId="5" r:id="rId4"/>
-    <sheet name="Template Burndown" sheetId="4" r:id="rId5"/>
-    <sheet name="Template" sheetId="1" r:id="rId6"/>
+    <sheet name="Tasks Sprint 2" sheetId="7" r:id="rId5"/>
+    <sheet name="Template Burndown" sheetId="4" r:id="rId6"/>
+    <sheet name="Template" sheetId="1" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Tasks Sprint 1'!$A$1:$H$21</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Tasks Sprint 2'!$A$1:$H$21</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Timeline!$J$9:$N$144</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -32,9 +34,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="791" uniqueCount="406">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="808" uniqueCount="398">
   <si>
     <t>User Story ID</t>
   </si>
@@ -131,19 +131,10 @@
     <t>Wasn't given to us - needed Game class to be well formed</t>
   </si>
   <si>
-    <t>Unfinished in sprint 1</t>
-  </si>
-  <si>
     <t>Took about as much effort as expected</t>
   </si>
   <si>
-    <t>Still haven't implemented Quitting at any time (not just at the end of a game)</t>
-  </si>
-  <si>
     <t>Card/Player impementation took some planning</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stats are available - DB connection is </t>
   </si>
   <si>
     <t>Simple to implement after round winner has been decided</t>
@@ -1227,36 +1218,6 @@
     <t>Who has won should be displayed each round</t>
   </si>
   <si>
-    <t>I want to be able to quit.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">As a human player, I want to be able to choose whether to play top trumps online or on the command line. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">As a human player, I want to be able to select an attribute on my active top trumps card. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">I want to be able to view statistics concerning past games and scores. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">As a human player I want to have the option of starting a new game after finishing one. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">As a human player, I want to be able to select the number of AI opponents. </t>
-  </si>
-  <si>
-    <t>As a user I want to see my top card.</t>
-  </si>
-  <si>
-    <t>Who has won should be displayed each round.</t>
-  </si>
-  <si>
-    <t>As a user I want to be able to view aggregate statistics of past games.</t>
-  </si>
-  <si>
-    <t>Acctual</t>
-  </si>
-  <si>
     <t>Plan</t>
   </si>
   <si>
@@ -1264,6 +1225,21 @@
   </si>
   <si>
     <t>Sprint 1 - Days</t>
+  </si>
+  <si>
+    <t>Pulls from database, shows only aggregated stats</t>
+  </si>
+  <si>
+    <t>Can quit at end of every round, or start of every game</t>
+  </si>
+  <si>
+    <t>Stats are available - DB connection is stable (assumed set up is complete beforehand)</t>
+  </si>
+  <si>
+    <t>Actual</t>
+  </si>
+  <si>
+    <t>As a user I want to be able to view aggregate statistics of past games Priority: 8 Cost 4</t>
   </si>
 </sst>
 </file>
@@ -2352,7 +2328,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Acctual</c:v>
+                  <c:v>Actual</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3359,8 +3335,8 @@
       <xdr:rowOff>18514</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>587840</xdr:colOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>218046</xdr:colOff>
       <xdr:row>62</xdr:row>
       <xdr:rowOff>178782</xdr:rowOff>
     </xdr:to>
@@ -3403,16 +3379,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>481852</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>124384</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>829235</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>1118</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>44824</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>168088</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>156881</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3758,7 +3734,7 @@
   <dimension ref="A1:N144"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3788,10 +3764,10 @@
     <row r="2" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="39"/>
       <c r="B2" s="43" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C2" s="44" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D2" s="74"/>
       <c r="E2" s="71"/>
@@ -3799,7 +3775,7 @@
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="39"/>
       <c r="B3" s="45" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C3" s="46">
         <v>0</v>
@@ -3810,10 +3786,10 @@
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="39"/>
       <c r="B4" s="47" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C4" s="48" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D4" s="74"/>
       <c r="E4" s="71"/>
@@ -3821,10 +3797,10 @@
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="39"/>
       <c r="B5" s="47" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C5" s="48" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D5" s="74"/>
       <c r="E5" s="71"/>
@@ -3832,10 +3808,10 @@
     <row r="6" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="39"/>
       <c r="B6" s="49" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C6" s="50" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D6" s="74"/>
       <c r="E6" s="71"/>
@@ -3850,118 +3826,118 @@
     <row r="8" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="55" t="s">
+        <v>81</v>
+      </c>
+      <c r="C9" s="56" t="s">
+        <v>82</v>
+      </c>
+      <c r="D9" s="56" t="s">
+        <v>379</v>
+      </c>
+      <c r="E9" s="57" t="s">
+        <v>83</v>
+      </c>
+      <c r="F9" s="57" t="s">
         <v>84</v>
       </c>
-      <c r="C9" s="56" t="s">
+      <c r="G9" s="58" t="s">
         <v>85</v>
       </c>
-      <c r="D9" s="56" t="s">
-        <v>382</v>
-      </c>
-      <c r="E9" s="57" t="s">
-        <v>86</v>
-      </c>
-      <c r="F9" s="57" t="s">
-        <v>87</v>
-      </c>
-      <c r="G9" s="58" t="s">
-        <v>88</v>
-      </c>
       <c r="J9" t="s">
+        <v>374</v>
+      </c>
+      <c r="K9" t="s">
+        <v>375</v>
+      </c>
+      <c r="L9" t="s">
+        <v>376</v>
+      </c>
+      <c r="M9" t="s">
         <v>377</v>
       </c>
-      <c r="K9" t="s">
+      <c r="N9" t="s">
         <v>378</v>
-      </c>
-      <c r="L9" t="s">
-        <v>379</v>
-      </c>
-      <c r="M9" t="s">
-        <v>380</v>
-      </c>
-      <c r="N9" t="s">
-        <v>381</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B10" s="45" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C10" s="53">
         <v>43847</v>
       </c>
       <c r="D10" s="69" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="E10" s="54" t="str">
         <f ca="1">IF(TODAY() &gt;= C10,"X", "")</f>
         <v>X</v>
       </c>
       <c r="F10" s="54" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="G10" s="59" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="J10">
         <v>1</v>
       </c>
       <c r="K10" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="L10" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="M10" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="N10" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B11" s="60" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C11" s="51">
         <v>43848</v>
       </c>
       <c r="D11" s="69" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="E11" s="54" t="str">
         <f t="shared" ref="E11:E41" ca="1" si="0">IF(TODAY() &gt;= C11,"X", "")</f>
         <v>X</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="G11" s="61"/>
       <c r="J11">
         <v>2</v>
       </c>
       <c r="K11" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="L11" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="M11" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="N11" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B12" s="60" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C12" s="51">
         <v>43849</v>
       </c>
       <c r="D12" s="69" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="E12" s="54" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -3973,16 +3949,16 @@
         <v>3</v>
       </c>
       <c r="K12" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="L12" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="M12" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="N12" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
@@ -3991,30 +3967,30 @@
         <v>43850</v>
       </c>
       <c r="D13" s="69" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="E13" s="54" t="str">
         <f t="shared" ca="1" si="0"/>
         <v>X</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="G13" s="61"/>
       <c r="J13">
         <v>4</v>
       </c>
       <c r="K13" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="L13" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="M13" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="N13" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="45" x14ac:dyDescent="0.25">
@@ -4023,30 +3999,30 @@
         <v>43851</v>
       </c>
       <c r="D14" s="69" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="E14" s="54" t="str">
         <f t="shared" ca="1" si="0"/>
         <v>X</v>
       </c>
       <c r="F14" s="68" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="G14" s="61"/>
       <c r="J14">
         <v>5</v>
       </c>
       <c r="K14" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="L14" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="M14" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="N14" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="30" x14ac:dyDescent="0.25">
@@ -4055,30 +4031,30 @@
         <v>43852</v>
       </c>
       <c r="D15" s="69" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="E15" s="54" t="str">
         <f t="shared" ca="1" si="0"/>
         <v>X</v>
       </c>
       <c r="F15" s="68" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="G15" s="61"/>
       <c r="J15">
         <v>6</v>
       </c>
       <c r="K15" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="L15" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="M15" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="N15" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="30" x14ac:dyDescent="0.25">
@@ -4087,30 +4063,30 @@
         <v>43853</v>
       </c>
       <c r="D16" s="69" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="E16" s="54" t="str">
         <f t="shared" ca="1" si="0"/>
         <v>X</v>
       </c>
       <c r="F16" s="68" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="G16" s="61"/>
       <c r="J16">
         <v>7</v>
       </c>
       <c r="K16" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="L16" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="M16" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="N16" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.25">
@@ -4119,7 +4095,7 @@
         <v>43854</v>
       </c>
       <c r="D17" s="69" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="E17" s="54" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -4131,61 +4107,61 @@
         <v>8</v>
       </c>
       <c r="K17" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="L17" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="M17" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="N17" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B18" s="60" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C18" s="51">
         <v>43855</v>
       </c>
       <c r="D18" s="69" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="E18" s="54" t="str">
         <f t="shared" ca="1" si="0"/>
         <v>X</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="G18" s="61"/>
       <c r="J18">
         <v>9</v>
       </c>
       <c r="K18" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="L18" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="M18" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="N18" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B19" s="60" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C19" s="51">
         <v>43856</v>
       </c>
       <c r="D19" s="69" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="E19" s="54" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -4197,16 +4173,16 @@
         <v>10</v>
       </c>
       <c r="K19" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="L19" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="M19" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="N19" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.25">
@@ -4215,7 +4191,7 @@
         <v>43857</v>
       </c>
       <c r="D20" s="69" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="E20" s="54" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -4227,16 +4203,16 @@
         <v>11</v>
       </c>
       <c r="K20" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="L20" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="M20" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="N20" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.25">
@@ -4245,30 +4221,30 @@
         <v>43858</v>
       </c>
       <c r="D21" s="69" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="E21" s="54" t="str">
         <f t="shared" ca="1" si="0"/>
         <v>X</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="G21" s="61"/>
       <c r="J21">
         <v>12</v>
       </c>
       <c r="K21" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="L21" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="M21" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="N21" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.25">
@@ -4277,32 +4253,32 @@
         <v>43859</v>
       </c>
       <c r="D22" s="69" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="E22" s="54" t="str">
         <f t="shared" ca="1" si="0"/>
         <v>X</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="G22" s="61" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="J22">
         <v>13</v>
       </c>
       <c r="K22" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="L22" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="M22" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="N22" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.25">
@@ -4311,11 +4287,11 @@
         <v>43860</v>
       </c>
       <c r="D23" s="69" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="E23" s="54" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="F23" s="2"/>
       <c r="G23" s="61"/>
@@ -4323,31 +4299,31 @@
         <v>14</v>
       </c>
       <c r="K23" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="L23" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="M23" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="N23" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B24" s="62" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C24" s="51">
         <v>43861</v>
       </c>
       <c r="D24" s="69" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="E24" s="54" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="F24" s="2"/>
       <c r="G24" s="61"/>
@@ -4355,27 +4331,27 @@
         <v>15</v>
       </c>
       <c r="K24" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="L24" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="M24" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="N24" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B25" s="60" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C25" s="52">
         <v>43862</v>
       </c>
       <c r="D25" s="70" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="E25" s="54" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -4387,27 +4363,27 @@
         <v>16</v>
       </c>
       <c r="K25" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="L25" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="M25" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="N25" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B26" s="60" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C26" s="52">
         <v>43863</v>
       </c>
       <c r="D26" s="70" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="E26" s="54" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -4419,27 +4395,27 @@
         <v>17</v>
       </c>
       <c r="K26" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="L26" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="M26" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="N26" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B27" s="62" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C27" s="52">
         <v>43864</v>
       </c>
       <c r="D27" s="70" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="E27" s="54" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -4451,16 +4427,16 @@
         <v>18</v>
       </c>
       <c r="K27" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="L27" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="M27" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="N27" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.25">
@@ -4469,7 +4445,7 @@
         <v>43865</v>
       </c>
       <c r="D28" s="70" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="E28" s="54" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -4481,16 +4457,16 @@
         <v>19</v>
       </c>
       <c r="K28" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="L28" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="M28" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="N28" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.25">
@@ -4499,7 +4475,7 @@
         <v>43866</v>
       </c>
       <c r="D29" s="70" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="E29" s="54" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -4511,16 +4487,16 @@
         <v>20</v>
       </c>
       <c r="K29" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="L29" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="M29" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="N29" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
     </row>
     <row r="30" spans="2:14" x14ac:dyDescent="0.25">
@@ -4529,7 +4505,7 @@
         <v>43867</v>
       </c>
       <c r="D30" s="70" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="E30" s="54" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -4541,16 +4517,16 @@
         <v>21</v>
       </c>
       <c r="K30" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="L30" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="M30" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="N30" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
     </row>
     <row r="31" spans="2:14" x14ac:dyDescent="0.25">
@@ -4559,7 +4535,7 @@
         <v>43868</v>
       </c>
       <c r="D31" s="70" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="E31" s="54" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -4571,27 +4547,27 @@
         <v>22</v>
       </c>
       <c r="K31" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="L31" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="M31" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="N31" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
     </row>
     <row r="32" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B32" s="60" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C32" s="52">
         <v>43869</v>
       </c>
       <c r="D32" s="70" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="E32" s="54" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -4603,27 +4579,27 @@
         <v>23</v>
       </c>
       <c r="K32" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="L32" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="M32" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="N32" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
     </row>
     <row r="33" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B33" s="60" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C33" s="52">
         <v>43870</v>
       </c>
       <c r="D33" s="70" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="E33" s="54" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -4635,16 +4611,16 @@
         <v>24</v>
       </c>
       <c r="K33" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="L33" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="M33" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="N33" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
     </row>
     <row r="34" spans="2:14" x14ac:dyDescent="0.25">
@@ -4653,7 +4629,7 @@
         <v>43871</v>
       </c>
       <c r="D34" s="70" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="E34" s="54" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -4665,16 +4641,16 @@
         <v>25</v>
       </c>
       <c r="K34" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="L34" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="M34" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="N34" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
     </row>
     <row r="35" spans="2:14" x14ac:dyDescent="0.25">
@@ -4683,7 +4659,7 @@
         <v>43872</v>
       </c>
       <c r="D35" s="70" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="E35" s="54" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -4695,16 +4671,16 @@
         <v>26</v>
       </c>
       <c r="K35" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="L35" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="M35" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="N35" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
     </row>
     <row r="36" spans="2:14" x14ac:dyDescent="0.25">
@@ -4713,7 +4689,7 @@
         <v>43873</v>
       </c>
       <c r="D36" s="70" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="E36" s="54" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -4725,16 +4701,16 @@
         <v>27</v>
       </c>
       <c r="K36" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="L36" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="M36" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="N36" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
     </row>
     <row r="37" spans="2:14" x14ac:dyDescent="0.25">
@@ -4743,7 +4719,7 @@
         <v>43874</v>
       </c>
       <c r="D37" s="70" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="E37" s="54" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -4755,27 +4731,27 @@
         <v>28</v>
       </c>
       <c r="K37" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="L37" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="M37" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="N37" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
     </row>
     <row r="38" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B38" s="62" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C38" s="52">
         <v>43875</v>
       </c>
       <c r="D38" s="70" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="E38" s="54" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -4787,27 +4763,27 @@
         <v>29</v>
       </c>
       <c r="K38" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="L38" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="M38" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="N38" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
     </row>
     <row r="39" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B39" s="60" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C39" s="52">
         <v>43876</v>
       </c>
       <c r="D39" s="70" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="E39" s="54" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -4819,27 +4795,27 @@
         <v>30</v>
       </c>
       <c r="K39" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="L39" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="M39" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="N39" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
     </row>
     <row r="40" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B40" s="60" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C40" s="52">
         <v>43877</v>
       </c>
       <c r="D40" s="70" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="E40" s="54" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -4851,27 +4827,27 @@
         <v>31</v>
       </c>
       <c r="K40" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="L40" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="M40" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="N40" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
     </row>
     <row r="41" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B41" s="64" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C41" s="65">
         <v>43878</v>
       </c>
       <c r="D41" s="70" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="E41" s="54" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -4883,16 +4859,16 @@
         <v>32</v>
       </c>
       <c r="K41" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="L41" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="M41" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="N41" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
     </row>
     <row r="42" spans="2:14" x14ac:dyDescent="0.25">
@@ -4900,16 +4876,16 @@
         <v>33</v>
       </c>
       <c r="K42" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="L42" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="M42" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="N42" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="43" spans="2:14" x14ac:dyDescent="0.25">
@@ -4917,16 +4893,16 @@
         <v>34</v>
       </c>
       <c r="K43" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="L43" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="M43" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="N43" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="44" spans="2:14" x14ac:dyDescent="0.25">
@@ -4934,16 +4910,16 @@
         <v>35</v>
       </c>
       <c r="K44" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="L44" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="M44" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="N44" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="45" spans="2:14" x14ac:dyDescent="0.25">
@@ -4951,16 +4927,16 @@
         <v>36</v>
       </c>
       <c r="K45" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="L45" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="M45" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="N45" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="46" spans="2:14" x14ac:dyDescent="0.25">
@@ -4968,16 +4944,16 @@
         <v>37</v>
       </c>
       <c r="K46" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="L46" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="M46" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="N46" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="47" spans="2:14" x14ac:dyDescent="0.25">
@@ -4985,16 +4961,16 @@
         <v>38</v>
       </c>
       <c r="K47" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="L47" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="M47" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="N47" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
     </row>
     <row r="48" spans="2:14" x14ac:dyDescent="0.25">
@@ -5002,16 +4978,16 @@
         <v>39</v>
       </c>
       <c r="K48" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="L48" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="M48" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="N48" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
     </row>
     <row r="49" spans="10:14" x14ac:dyDescent="0.25">
@@ -5019,16 +4995,16 @@
         <v>40</v>
       </c>
       <c r="K49" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="L49" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="M49" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="N49" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="50" spans="10:14" x14ac:dyDescent="0.25">
@@ -5036,16 +5012,16 @@
         <v>41</v>
       </c>
       <c r="K50" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="L50" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="M50" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="N50" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="51" spans="10:14" x14ac:dyDescent="0.25">
@@ -5053,16 +5029,16 @@
         <v>42</v>
       </c>
       <c r="K51" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="L51" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="M51" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="N51" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
     </row>
     <row r="52" spans="10:14" x14ac:dyDescent="0.25">
@@ -5070,16 +5046,16 @@
         <v>43</v>
       </c>
       <c r="K52" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="L52" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="M52" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="N52" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
     </row>
     <row r="53" spans="10:14" x14ac:dyDescent="0.25">
@@ -5087,16 +5063,16 @@
         <v>44</v>
       </c>
       <c r="K53" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="L53" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="M53" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="N53" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="54" spans="10:14" x14ac:dyDescent="0.25">
@@ -5104,16 +5080,16 @@
         <v>45</v>
       </c>
       <c r="K54" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="L54" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="M54" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="N54" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="55" spans="10:14" x14ac:dyDescent="0.25">
@@ -5121,16 +5097,16 @@
         <v>46</v>
       </c>
       <c r="K55" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="L55" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="M55" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="N55" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="56" spans="10:14" x14ac:dyDescent="0.25">
@@ -5138,16 +5114,16 @@
         <v>47</v>
       </c>
       <c r="K56" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="L56" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="M56" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="N56" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="57" spans="10:14" x14ac:dyDescent="0.25">
@@ -5155,16 +5131,16 @@
         <v>48</v>
       </c>
       <c r="K57" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="L57" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="M57" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="N57" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="58" spans="10:14" x14ac:dyDescent="0.25">
@@ -5172,16 +5148,16 @@
         <v>49</v>
       </c>
       <c r="K58" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="L58" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="M58" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="N58" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="59" spans="10:14" x14ac:dyDescent="0.25">
@@ -5189,16 +5165,16 @@
         <v>50</v>
       </c>
       <c r="K59" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="L59" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="M59" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="N59" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="60" spans="10:14" x14ac:dyDescent="0.25">
@@ -5206,16 +5182,16 @@
         <v>51</v>
       </c>
       <c r="K60" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="L60" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="M60" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="N60" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="61" spans="10:14" x14ac:dyDescent="0.25">
@@ -5223,16 +5199,16 @@
         <v>52</v>
       </c>
       <c r="K61" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="L61" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="M61" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="N61" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="62" spans="10:14" x14ac:dyDescent="0.25">
@@ -5240,16 +5216,16 @@
         <v>53</v>
       </c>
       <c r="K62" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="L62" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="M62" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="N62" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
     </row>
     <row r="63" spans="10:14" x14ac:dyDescent="0.25">
@@ -5257,16 +5233,16 @@
         <v>54</v>
       </c>
       <c r="K63" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="L63" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="M63" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="N63" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="64" spans="10:14" x14ac:dyDescent="0.25">
@@ -5274,16 +5250,16 @@
         <v>55</v>
       </c>
       <c r="K64" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="L64" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="M64" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="N64" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
     </row>
     <row r="65" spans="10:14" x14ac:dyDescent="0.25">
@@ -5291,16 +5267,16 @@
         <v>56</v>
       </c>
       <c r="K65" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="L65" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="M65" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="N65" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="66" spans="10:14" x14ac:dyDescent="0.25">
@@ -5308,16 +5284,16 @@
         <v>57</v>
       </c>
       <c r="K66" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="L66" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="M66" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="N66" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="67" spans="10:14" x14ac:dyDescent="0.25">
@@ -5325,16 +5301,16 @@
         <v>58</v>
       </c>
       <c r="K67" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="L67" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="M67" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="N67" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="68" spans="10:14" x14ac:dyDescent="0.25">
@@ -5342,16 +5318,16 @@
         <v>59</v>
       </c>
       <c r="K68" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="L68" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="M68" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="N68" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
     </row>
     <row r="69" spans="10:14" x14ac:dyDescent="0.25">
@@ -5359,16 +5335,16 @@
         <v>60</v>
       </c>
       <c r="K69" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="L69" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="M69" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="N69" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="70" spans="10:14" x14ac:dyDescent="0.25">
@@ -5376,16 +5352,16 @@
         <v>61</v>
       </c>
       <c r="K70" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="L70" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="M70" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="N70" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="71" spans="10:14" x14ac:dyDescent="0.25">
@@ -5393,16 +5369,16 @@
         <v>62</v>
       </c>
       <c r="K71" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="L71" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="M71" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="N71" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="72" spans="10:14" x14ac:dyDescent="0.25">
@@ -5410,16 +5386,16 @@
         <v>63</v>
       </c>
       <c r="K72" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="L72" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="M72" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="N72" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="73" spans="10:14" x14ac:dyDescent="0.25">
@@ -5427,16 +5403,16 @@
         <v>64</v>
       </c>
       <c r="K73" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="L73" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="M73" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="N73" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
     </row>
     <row r="74" spans="10:14" x14ac:dyDescent="0.25">
@@ -5444,16 +5420,16 @@
         <v>65</v>
       </c>
       <c r="K74" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="L74" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="M74" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="N74" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="75" spans="10:14" x14ac:dyDescent="0.25">
@@ -5461,16 +5437,16 @@
         <v>66</v>
       </c>
       <c r="K75" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="L75" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="M75" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="N75" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="76" spans="10:14" x14ac:dyDescent="0.25">
@@ -5478,16 +5454,16 @@
         <v>67</v>
       </c>
       <c r="K76" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="L76" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="M76" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="N76" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="77" spans="10:14" x14ac:dyDescent="0.25">
@@ -5495,16 +5471,16 @@
         <v>68</v>
       </c>
       <c r="K77" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="L77" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="M77" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="N77" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="78" spans="10:14" x14ac:dyDescent="0.25">
@@ -5512,16 +5488,16 @@
         <v>69</v>
       </c>
       <c r="K78" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="L78" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="M78" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="N78" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="79" spans="10:14" x14ac:dyDescent="0.25">
@@ -5529,16 +5505,16 @@
         <v>70</v>
       </c>
       <c r="K79" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="L79" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="M79" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="N79" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="80" spans="10:14" x14ac:dyDescent="0.25">
@@ -5546,16 +5522,16 @@
         <v>71</v>
       </c>
       <c r="K80" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="L80" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="M80" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="N80" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="81" spans="10:14" x14ac:dyDescent="0.25">
@@ -5563,16 +5539,16 @@
         <v>72</v>
       </c>
       <c r="K81" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="L81" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="M81" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="N81" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="82" spans="10:14" x14ac:dyDescent="0.25">
@@ -5580,16 +5556,16 @@
         <v>73</v>
       </c>
       <c r="K82" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="L82" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="M82" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="N82" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
     <row r="83" spans="10:14" x14ac:dyDescent="0.25">
@@ -5597,16 +5573,16 @@
         <v>74</v>
       </c>
       <c r="K83" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="L83" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="M83" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="N83" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="84" spans="10:14" x14ac:dyDescent="0.25">
@@ -5614,16 +5590,16 @@
         <v>75</v>
       </c>
       <c r="K84" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="L84" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="M84" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="N84" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="85" spans="10:14" x14ac:dyDescent="0.25">
@@ -5631,16 +5607,16 @@
         <v>76</v>
       </c>
       <c r="K85" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="L85" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="M85" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="N85" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="86" spans="10:14" x14ac:dyDescent="0.25">
@@ -5648,16 +5624,16 @@
         <v>77</v>
       </c>
       <c r="K86" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="L86" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="M86" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="N86" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="87" spans="10:14" x14ac:dyDescent="0.25">
@@ -5665,16 +5641,16 @@
         <v>78</v>
       </c>
       <c r="K87" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="L87" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="M87" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="N87" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="88" spans="10:14" x14ac:dyDescent="0.25">
@@ -5682,16 +5658,16 @@
         <v>79</v>
       </c>
       <c r="K88" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="L88" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="M88" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="N88" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="89" spans="10:14" x14ac:dyDescent="0.25">
@@ -5699,16 +5675,16 @@
         <v>80</v>
       </c>
       <c r="K89" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="L89" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="M89" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="N89" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="90" spans="10:14" x14ac:dyDescent="0.25">
@@ -5716,16 +5692,16 @@
         <v>81</v>
       </c>
       <c r="K90" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="L90" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="M90" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="N90" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="91" spans="10:14" x14ac:dyDescent="0.25">
@@ -5733,16 +5709,16 @@
         <v>82</v>
       </c>
       <c r="K91" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="L91" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="M91" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="N91" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="92" spans="10:14" x14ac:dyDescent="0.25">
@@ -5750,16 +5726,16 @@
         <v>83</v>
       </c>
       <c r="K92" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="L92" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="M92" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="N92" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="93" spans="10:14" x14ac:dyDescent="0.25">
@@ -5767,16 +5743,16 @@
         <v>84</v>
       </c>
       <c r="K93" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="L93" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="M93" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="N93" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="94" spans="10:14" x14ac:dyDescent="0.25">
@@ -5784,16 +5760,16 @@
         <v>85</v>
       </c>
       <c r="K94" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="L94" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="M94" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="N94" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="95" spans="10:14" x14ac:dyDescent="0.25">
@@ -5801,16 +5777,16 @@
         <v>86</v>
       </c>
       <c r="K95" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="L95" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="M95" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="N95" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="96" spans="10:14" x14ac:dyDescent="0.25">
@@ -5818,16 +5794,16 @@
         <v>87</v>
       </c>
       <c r="K96" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="L96" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="M96" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="N96" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="97" spans="10:14" x14ac:dyDescent="0.25">
@@ -5835,16 +5811,16 @@
         <v>88</v>
       </c>
       <c r="K97" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="L97" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="M97" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="N97" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="98" spans="10:14" x14ac:dyDescent="0.25">
@@ -5852,16 +5828,16 @@
         <v>89</v>
       </c>
       <c r="K98" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="L98" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="M98" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="N98" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="99" spans="10:14" x14ac:dyDescent="0.25">
@@ -5869,16 +5845,16 @@
         <v>90</v>
       </c>
       <c r="K99" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="L99" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="M99" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="N99" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="100" spans="10:14" x14ac:dyDescent="0.25">
@@ -5886,16 +5862,16 @@
         <v>91</v>
       </c>
       <c r="K100" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="L100" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="M100" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="N100" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="101" spans="10:14" x14ac:dyDescent="0.25">
@@ -5903,16 +5879,16 @@
         <v>92</v>
       </c>
       <c r="K101" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="L101" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="M101" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="N101" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="102" spans="10:14" x14ac:dyDescent="0.25">
@@ -5920,16 +5896,16 @@
         <v>93</v>
       </c>
       <c r="K102" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="L102" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="M102" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="N102" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="103" spans="10:14" x14ac:dyDescent="0.25">
@@ -5937,16 +5913,16 @@
         <v>94</v>
       </c>
       <c r="K103" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="L103" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="M103" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="N103" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="104" spans="10:14" x14ac:dyDescent="0.25">
@@ -5954,16 +5930,16 @@
         <v>95</v>
       </c>
       <c r="K104" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="L104" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="M104" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="N104" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="105" spans="10:14" x14ac:dyDescent="0.25">
@@ -5971,16 +5947,16 @@
         <v>96</v>
       </c>
       <c r="K105" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="L105" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="M105" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="N105" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="106" spans="10:14" x14ac:dyDescent="0.25">
@@ -5988,16 +5964,16 @@
         <v>97</v>
       </c>
       <c r="K106" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="L106" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="M106" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="N106" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="107" spans="10:14" x14ac:dyDescent="0.25">
@@ -6005,16 +5981,16 @@
         <v>98</v>
       </c>
       <c r="K107" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="L107" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="M107" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="N107" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="108" spans="10:14" x14ac:dyDescent="0.25">
@@ -6022,16 +5998,16 @@
         <v>99</v>
       </c>
       <c r="K108" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="L108" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="M108" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="N108" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="109" spans="10:14" x14ac:dyDescent="0.25">
@@ -6039,16 +6015,16 @@
         <v>100</v>
       </c>
       <c r="K109" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="L109" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="M109" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="N109" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="110" spans="10:14" x14ac:dyDescent="0.25">
@@ -6056,16 +6032,16 @@
         <v>101</v>
       </c>
       <c r="K110" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="L110" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="M110" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="N110" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="111" spans="10:14" x14ac:dyDescent="0.25">
@@ -6073,16 +6049,16 @@
         <v>102</v>
       </c>
       <c r="K111" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="L111" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="M111" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="N111" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="112" spans="10:14" x14ac:dyDescent="0.25">
@@ -6090,16 +6066,16 @@
         <v>103</v>
       </c>
       <c r="K112" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="L112" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="M112" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="N112" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="113" spans="10:14" x14ac:dyDescent="0.25">
@@ -6107,16 +6083,16 @@
         <v>104</v>
       </c>
       <c r="K113" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="L113" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="M113" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="N113" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="114" spans="10:14" x14ac:dyDescent="0.25">
@@ -6124,16 +6100,16 @@
         <v>105</v>
       </c>
       <c r="K114" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="L114" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="M114" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="N114" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="115" spans="10:14" x14ac:dyDescent="0.25">
@@ -6141,16 +6117,16 @@
         <v>106</v>
       </c>
       <c r="K115" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="L115" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="M115" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="N115" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="116" spans="10:14" x14ac:dyDescent="0.25">
@@ -6158,16 +6134,16 @@
         <v>107</v>
       </c>
       <c r="K116" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="L116" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="M116" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="N116" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="117" spans="10:14" x14ac:dyDescent="0.25">
@@ -6175,16 +6151,16 @@
         <v>108</v>
       </c>
       <c r="K117" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="L117" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="M117" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="N117" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="118" spans="10:14" x14ac:dyDescent="0.25">
@@ -6192,16 +6168,16 @@
         <v>109</v>
       </c>
       <c r="K118" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="L118" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="M118" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="N118" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="119" spans="10:14" x14ac:dyDescent="0.25">
@@ -6209,16 +6185,16 @@
         <v>110</v>
       </c>
       <c r="K119" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="L119" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="M119" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="N119" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="120" spans="10:14" x14ac:dyDescent="0.25">
@@ -6226,16 +6202,16 @@
         <v>111</v>
       </c>
       <c r="K120" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="L120" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="M120" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="N120" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="121" spans="10:14" x14ac:dyDescent="0.25">
@@ -6243,16 +6219,16 @@
         <v>112</v>
       </c>
       <c r="K121" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="L121" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="M121" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="N121" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="122" spans="10:14" x14ac:dyDescent="0.25">
@@ -6260,16 +6236,16 @@
         <v>113</v>
       </c>
       <c r="K122" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="L122" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="M122" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="N122" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="123" spans="10:14" x14ac:dyDescent="0.25">
@@ -6277,16 +6253,16 @@
         <v>114</v>
       </c>
       <c r="K123" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="L123" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="M123" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="N123" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="124" spans="10:14" x14ac:dyDescent="0.25">
@@ -6294,16 +6270,16 @@
         <v>115</v>
       </c>
       <c r="K124" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="L124" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="M124" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="N124" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="125" spans="10:14" x14ac:dyDescent="0.25">
@@ -6311,16 +6287,16 @@
         <v>116</v>
       </c>
       <c r="K125" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="L125" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="M125" t="s">
+        <v>133</v>
+      </c>
+      <c r="N125" t="s">
         <v>136</v>
-      </c>
-      <c r="N125" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="126" spans="10:14" x14ac:dyDescent="0.25">
@@ -6328,16 +6304,16 @@
         <v>117</v>
       </c>
       <c r="K126" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="L126" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="M126" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="N126" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="127" spans="10:14" x14ac:dyDescent="0.25">
@@ -6345,16 +6321,16 @@
         <v>118</v>
       </c>
       <c r="K127" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="L127" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="M127" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="N127" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="128" spans="10:14" x14ac:dyDescent="0.25">
@@ -6362,16 +6338,16 @@
         <v>119</v>
       </c>
       <c r="K128" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="L128" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="M128" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="N128" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="129" spans="10:14" x14ac:dyDescent="0.25">
@@ -6379,16 +6355,16 @@
         <v>120</v>
       </c>
       <c r="K129" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="L129" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="M129" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="N129" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="130" spans="10:14" x14ac:dyDescent="0.25">
@@ -6396,16 +6372,16 @@
         <v>121</v>
       </c>
       <c r="K130" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="L130" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="M130" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="N130" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="131" spans="10:14" x14ac:dyDescent="0.25">
@@ -6413,16 +6389,16 @@
         <v>122</v>
       </c>
       <c r="K131" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="L131" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="M131" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="N131" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="132" spans="10:14" x14ac:dyDescent="0.25">
@@ -6430,16 +6406,16 @@
         <v>123</v>
       </c>
       <c r="K132" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="L132" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="M132" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="N132" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="133" spans="10:14" x14ac:dyDescent="0.25">
@@ -6447,16 +6423,16 @@
         <v>124</v>
       </c>
       <c r="K133" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="L133" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="M133" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="N133" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="134" spans="10:14" x14ac:dyDescent="0.25">
@@ -6464,16 +6440,16 @@
         <v>125</v>
       </c>
       <c r="K134" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="L134" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="M134" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="N134" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="135" spans="10:14" x14ac:dyDescent="0.25">
@@ -6481,16 +6457,16 @@
         <v>126</v>
       </c>
       <c r="K135" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="L135" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="M135" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="N135" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="136" spans="10:14" x14ac:dyDescent="0.25">
@@ -6498,16 +6474,16 @@
         <v>127</v>
       </c>
       <c r="K136" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="L136" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="M136" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="N136" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="137" spans="10:14" x14ac:dyDescent="0.25">
@@ -6515,16 +6491,16 @@
         <v>128</v>
       </c>
       <c r="K137" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="L137" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="M137" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="N137" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="138" spans="10:14" x14ac:dyDescent="0.25">
@@ -6532,16 +6508,16 @@
         <v>129</v>
       </c>
       <c r="K138" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="L138" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="M138" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="N138" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="139" spans="10:14" x14ac:dyDescent="0.25">
@@ -6549,16 +6525,16 @@
         <v>130</v>
       </c>
       <c r="K139" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="L139" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="M139" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="N139" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="140" spans="10:14" x14ac:dyDescent="0.25">
@@ -6566,16 +6542,16 @@
         <v>131</v>
       </c>
       <c r="K140" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="L140" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="M140" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="N140" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="141" spans="10:14" x14ac:dyDescent="0.25">
@@ -6583,16 +6559,16 @@
         <v>132</v>
       </c>
       <c r="K141" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="L141" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="M141" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="N141" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="142" spans="10:14" x14ac:dyDescent="0.25">
@@ -6600,16 +6576,16 @@
         <v>133</v>
       </c>
       <c r="K142" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="L142" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="M142" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="N142" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="143" spans="10:14" x14ac:dyDescent="0.25">
@@ -6617,16 +6593,16 @@
         <v>134</v>
       </c>
       <c r="K143" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="L143" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="M143" t="s">
+        <v>88</v>
+      </c>
+      <c r="N143" t="s">
         <v>91</v>
-      </c>
-      <c r="N143" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="144" spans="10:14" x14ac:dyDescent="0.25">
@@ -6634,16 +6610,16 @@
         <v>135</v>
       </c>
       <c r="K144" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="L144" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="M144" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="N144" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -6665,7 +6641,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="A1:F10"/>
+      <selection activeCell="A2" sqref="A2:A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6683,13 +6659,13 @@
         <v>13</v>
       </c>
       <c r="B1" s="32" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C1" s="33" t="s">
         <v>10</v>
       </c>
       <c r="D1" s="33" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E1" s="33" t="s">
         <v>22</v>
@@ -6715,7 +6691,7 @@
         <v>10</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E2" s="12">
         <v>2</v>
@@ -6739,7 +6715,7 @@
         <v>10</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E3" s="21">
         <v>3</v>
@@ -6763,7 +6739,7 @@
         <v>8</v>
       </c>
       <c r="D4" s="21" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E4" s="21">
         <v>1</v>
@@ -6787,15 +6763,17 @@
         <v>6</v>
       </c>
       <c r="D5" s="21" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E5" s="21">
         <v>5</v>
       </c>
-      <c r="F5" s="21"/>
+      <c r="F5" s="21">
+        <v>7</v>
+      </c>
       <c r="G5" s="21"/>
       <c r="H5" s="23" t="s">
-        <v>29</v>
+        <v>393</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -6809,7 +6787,7 @@
         <v>10</v>
       </c>
       <c r="D6" s="21" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E6" s="21">
         <v>3</v>
@@ -6819,10 +6797,10 @@
       </c>
       <c r="G6" s="21"/>
       <c r="H6" s="23" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="22" t="s">
         <v>18</v>
       </c>
@@ -6833,15 +6811,17 @@
         <v>8</v>
       </c>
       <c r="D7" s="21" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E7" s="21">
         <v>1</v>
       </c>
-      <c r="F7" s="21"/>
+      <c r="F7" s="21">
+        <v>2</v>
+      </c>
       <c r="G7" s="21"/>
       <c r="H7" s="23" t="s">
-        <v>31</v>
+        <v>394</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.25">
@@ -6855,7 +6835,7 @@
         <v>7</v>
       </c>
       <c r="D8" s="21" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E8" s="21">
         <v>1</v>
@@ -6865,12 +6845,12 @@
       </c>
       <c r="G8" s="21"/>
       <c r="H8" s="23" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="22" t="s">
-        <v>20</v>
+        <v>397</v>
       </c>
       <c r="B9" s="29">
         <v>8</v>
@@ -6879,15 +6859,17 @@
         <v>8</v>
       </c>
       <c r="D9" s="21" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E9" s="21">
-        <v>1</v>
-      </c>
-      <c r="F9" s="21"/>
+        <v>4</v>
+      </c>
+      <c r="F9" s="21">
+        <v>5</v>
+      </c>
       <c r="G9" s="21"/>
       <c r="H9" s="23" t="s">
-        <v>33</v>
+        <v>395</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6901,7 +6883,7 @@
         <v>9</v>
       </c>
       <c r="D10" s="25" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E10" s="25">
         <v>1</v>
@@ -6911,7 +6893,7 @@
       </c>
       <c r="G10" s="25"/>
       <c r="H10" s="26" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -6924,7 +6906,7 @@
   <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6941,28 +6923,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>24</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -6973,10 +6955,10 @@
         <v>12</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2">
@@ -6997,10 +6979,10 @@
         <v>14</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2">
@@ -7021,10 +7003,10 @@
         <v>14</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
@@ -7039,7 +7021,7 @@
         <v>17</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -7061,7 +7043,7 @@
         <v>17</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -7077,7 +7059,7 @@
         <v>17</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -7093,7 +7075,7 @@
         <v>17</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -7109,7 +7091,7 @@
         <v>19</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
@@ -7131,7 +7113,7 @@
         <v>19</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -7167,10 +7149,10 @@
         <v>15</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2">
@@ -7191,11 +7173,12 @@
         <v>16</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2">
+        <f>INDEX('User Stories Sprint 1'!$E:$E,MATCH($A13,'User Stories Sprint 1'!$B:$B,0))</f>
         <v>5</v>
       </c>
       <c r="G13" s="2">
@@ -7211,7 +7194,7 @@
         <v>16</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
@@ -7227,7 +7210,7 @@
         <v>16</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
@@ -7243,7 +7226,7 @@
         <v>16</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
@@ -7259,7 +7242,7 @@
         <v>16</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
@@ -7275,7 +7258,7 @@
         <v>16</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
@@ -7291,7 +7274,7 @@
         <v>18</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
@@ -7301,7 +7284,7 @@
       </c>
       <c r="G19" s="2">
         <f>INDEX('User Stories Sprint 1'!$F:$F,MATCH($A19,'User Stories Sprint 1'!$B:$B,0))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H19" s="2"/>
     </row>
@@ -7313,7 +7296,7 @@
         <v>18</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
@@ -7329,28 +7312,28 @@
         <v>20</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2">
         <f>INDEX('User Stories Sprint 1'!$E:$E,MATCH($A21,'User Stories Sprint 1'!$B:$B,0))</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G21" s="2">
         <f>INDEX('User Stories Sprint 1'!$F:$F,MATCH($A21,'User Stories Sprint 1'!$B:$B,0))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H21" s="2"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F22">
         <f>SUM(F2:F21)</f>
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="G22">
         <f>SUM(G2:G21)</f>
-        <v>18</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -7368,7 +7351,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7386,13 +7369,13 @@
         <v>13</v>
       </c>
       <c r="B1" s="32" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C1" s="33" t="s">
         <v>10</v>
       </c>
       <c r="D1" s="33" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E1" s="33" t="s">
         <v>22</v>
@@ -7503,11 +7486,277 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2289136A-3240-48CC-95DE-2B454B379535}">
+  <dimension ref="A1:H22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" style="18" customWidth="1"/>
+    <col min="2" max="2" width="29.42578125" customWidth="1"/>
+    <col min="3" max="3" width="49.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.42578125" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" customWidth="1"/>
+    <col min="8" max="8" width="8.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="20"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="20"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="20"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="20"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="20"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="20"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="20"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="20"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="20"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="20"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="20"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="20"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="20"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="20"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="20"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="20"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="20"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="20"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="20"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="20"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F22">
+        <f>SUM(F2:F21)</f>
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <f>SUM(G2:G21)</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:H21" xr:uid="{9515D1DC-4AE1-4B79-A751-D444B917CA23}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H21">
+      <sortCondition ref="H1:H21"/>
+    </sortState>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59333514-8FD2-4190-8532-38CFA6C50E52}">
   <dimension ref="A1:N35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="R18" sqref="R18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7519,23 +7768,26 @@
     <col min="6" max="6" width="12.42578125" customWidth="1"/>
     <col min="7" max="7" width="9.140625" customWidth="1"/>
     <col min="8" max="8" width="14.7109375" customWidth="1"/>
+    <col min="12" max="12" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="75" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="76" t="s">
+        <v>386</v>
+      </c>
+      <c r="C1" s="75" t="s">
+        <v>387</v>
+      </c>
+      <c r="D1" s="75" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="76" t="s">
-        <v>389</v>
-      </c>
-      <c r="C1" s="75" t="s">
-        <v>390</v>
-      </c>
-      <c r="D1" s="75" t="s">
-        <v>38</v>
-      </c>
       <c r="E1" s="75" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -7543,10 +7795,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="D2" s="20">
         <v>2</v>
@@ -7560,10 +7812,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C3" s="20" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="D3" s="20">
         <v>3</v>
@@ -7577,7 +7829,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C4" s="20"/>
       <c r="D4" s="20"/>
@@ -7588,10 +7840,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="D5" s="20">
         <v>3</v>
@@ -7605,7 +7857,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C6" s="20"/>
       <c r="D6" s="20"/>
@@ -7616,7 +7868,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C7" s="20"/>
       <c r="D7" s="20"/>
@@ -7627,10 +7879,10 @@
         <v>4</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C8" s="20" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="D8" s="20">
         <v>1</v>
@@ -7644,7 +7896,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C9" s="20"/>
       <c r="D9" s="20"/>
@@ -7655,10 +7907,10 @@
         <v>4</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C10" s="20" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="D10" s="20">
         <v>1</v>
@@ -7672,10 +7924,10 @@
         <v>4</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C11" s="20" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="D11" s="20">
         <v>1</v>
@@ -7689,10 +7941,10 @@
         <v>5</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C12" s="20" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="D12" s="20">
         <v>5</v>
@@ -7706,7 +7958,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C13" s="20"/>
       <c r="D13" s="20"/>
@@ -7717,7 +7969,7 @@
         <v>5</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C14" s="20"/>
       <c r="D14" s="20"/>
@@ -7728,7 +7980,7 @@
         <v>5</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C15" s="20"/>
       <c r="D15" s="20"/>
@@ -7739,10 +7991,10 @@
         <v>6</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C16" s="20" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="D16" s="20">
         <v>1</v>
@@ -7756,7 +8008,7 @@
         <v>6</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C17" s="20"/>
       <c r="D17" s="20"/>
@@ -7767,7 +8019,7 @@
         <v>7</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C18" s="20"/>
       <c r="D18" s="20"/>
@@ -7778,7 +8030,7 @@
         <v>7</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C19" s="20"/>
       <c r="D19" s="20"/>
@@ -7789,10 +8041,10 @@
         <v>8</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C20" s="20" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="D20" s="20">
         <v>1</v>
@@ -7806,15 +8058,15 @@
         <v>9</v>
       </c>
       <c r="B21" s="78" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="C21" s="20"/>
       <c r="D21" s="20"/>
       <c r="E21" s="20"/>
     </row>
-    <row r="22" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="77" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="B22" s="78"/>
       <c r="C22" s="2"/>
@@ -7823,35 +8075,35 @@
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="H23" t="s">
-        <v>404</v>
+        <v>391</v>
       </c>
       <c r="L23" t="s">
-        <v>404</v>
+        <v>391</v>
       </c>
     </row>
     <row r="24" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H24" s="20" t="s">
-        <v>405</v>
+        <v>392</v>
       </c>
       <c r="I24" s="20" t="s">
-        <v>403</v>
+        <v>390</v>
       </c>
       <c r="J24" s="20" t="s">
-        <v>402</v>
+        <v>396</v>
       </c>
       <c r="L24" s="20" t="s">
-        <v>405</v>
+        <v>392</v>
       </c>
       <c r="M24" s="20" t="s">
-        <v>403</v>
+        <v>390</v>
       </c>
       <c r="N24" s="20" t="s">
-        <v>402</v>
+        <v>396</v>
       </c>
     </row>
     <row r="25" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="32" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B25" s="31" t="s">
         <v>13</v>
@@ -7860,7 +8112,7 @@
         <v>10</v>
       </c>
       <c r="D25" s="33" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E25" s="33" t="s">
         <v>22</v>
@@ -7887,18 +8139,18 @@
         <v>19</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="11">
         <v>1</v>
       </c>
       <c r="B26" s="27" t="s">
-        <v>394</v>
+        <v>12</v>
       </c>
       <c r="C26" s="12">
         <v>10</v>
       </c>
       <c r="D26" s="12" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E26" s="12">
         <v>2</v>
@@ -7906,8 +8158,8 @@
       <c r="F26" s="12">
         <v>1</v>
       </c>
-      <c r="H26" s="20">
-        <v>2</v>
+      <c r="H26" s="20" t="s">
+        <v>26</v>
       </c>
       <c r="I26" s="20">
         <v>16</v>
@@ -7925,18 +8177,18 @@
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="29">
         <v>2</v>
       </c>
       <c r="B27" s="22" t="s">
-        <v>398</v>
+        <v>14</v>
       </c>
       <c r="C27" s="21">
         <v>10</v>
       </c>
       <c r="D27" s="12" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E27" s="21">
         <v>3</v>
@@ -7944,8 +8196,8 @@
       <c r="F27" s="21">
         <v>2</v>
       </c>
-      <c r="H27" s="20">
-        <v>3</v>
+      <c r="H27" s="20" t="s">
+        <v>27</v>
       </c>
       <c r="I27" s="20">
         <v>13</v>
@@ -7963,18 +8215,18 @@
         <v>16</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="29">
         <v>3</v>
       </c>
       <c r="B28" s="22" t="s">
-        <v>397</v>
+        <v>15</v>
       </c>
       <c r="C28" s="21">
         <v>8</v>
       </c>
       <c r="D28" s="21" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E28" s="21">
         <v>1</v>
@@ -7982,8 +8234,8 @@
       <c r="F28" s="21">
         <v>3</v>
       </c>
-      <c r="H28" s="20">
-        <v>4</v>
+      <c r="H28" s="20" t="s">
+        <v>28</v>
       </c>
       <c r="I28" s="20">
         <v>12</v>
@@ -8001,27 +8253,27 @@
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="29">
         <v>4</v>
       </c>
       <c r="B29" s="22" t="s">
-        <v>396</v>
+        <v>16</v>
       </c>
       <c r="C29" s="21">
         <v>6</v>
       </c>
       <c r="D29" s="21" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E29" s="21">
         <v>5</v>
       </c>
       <c r="F29" s="21">
-        <v>5</v>
-      </c>
-      <c r="H29" s="20">
-        <v>5</v>
+        <v>7</v>
+      </c>
+      <c r="H29" s="20" t="s">
+        <v>393</v>
       </c>
       <c r="I29" s="20">
         <v>7</v>
@@ -8039,18 +8291,18 @@
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="29">
         <v>5</v>
       </c>
       <c r="B30" s="22" t="s">
-        <v>395</v>
+        <v>17</v>
       </c>
       <c r="C30" s="21">
         <v>10</v>
       </c>
       <c r="D30" s="21" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E30" s="21">
         <v>3</v>
@@ -8058,8 +8310,8 @@
       <c r="F30" s="21">
         <v>3</v>
       </c>
-      <c r="H30" s="20">
-        <v>6</v>
+      <c r="H30" s="20" t="s">
+        <v>29</v>
       </c>
       <c r="I30" s="20">
         <v>4</v>
@@ -8077,27 +8329,27 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="29">
         <v>6</v>
       </c>
       <c r="B31" s="22" t="s">
-        <v>393</v>
+        <v>18</v>
       </c>
       <c r="C31" s="21">
         <v>8</v>
       </c>
       <c r="D31" s="21" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E31" s="21">
         <v>1</v>
       </c>
       <c r="F31" s="21">
-        <v>1</v>
-      </c>
-      <c r="H31" s="20">
-        <v>7</v>
+        <v>2</v>
+      </c>
+      <c r="H31" s="20" t="s">
+        <v>394</v>
       </c>
       <c r="I31" s="20">
         <v>3</v>
@@ -8115,18 +8367,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="29">
         <v>7</v>
       </c>
       <c r="B32" s="22" t="s">
-        <v>399</v>
+        <v>19</v>
       </c>
       <c r="C32" s="21">
         <v>7</v>
       </c>
       <c r="D32" s="21" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E32" s="21">
         <v>1</v>
@@ -8134,8 +8386,8 @@
       <c r="F32" s="21">
         <v>2</v>
       </c>
-      <c r="H32" s="20">
-        <v>8</v>
+      <c r="H32" s="20" t="s">
+        <v>30</v>
       </c>
       <c r="I32" s="20">
         <v>2</v>
@@ -8153,27 +8405,27 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="29">
         <v>8</v>
       </c>
       <c r="B33" s="22" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="C33" s="21">
         <v>8</v>
       </c>
       <c r="D33" s="21" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E33" s="21">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F33" s="21">
-        <v>1</v>
-      </c>
-      <c r="H33" s="20">
-        <v>9</v>
+        <v>5</v>
+      </c>
+      <c r="H33" s="20" t="s">
+        <v>395</v>
       </c>
       <c r="I33" s="20">
         <v>1</v>
@@ -8191,18 +8443,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:14" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="30">
         <v>9</v>
       </c>
       <c r="B34" s="24" t="s">
-        <v>400</v>
+        <v>21</v>
       </c>
       <c r="C34" s="25">
         <v>9</v>
       </c>
       <c r="D34" s="25" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E34" s="25">
         <v>1</v>
@@ -8210,8 +8462,8 @@
       <c r="F34" s="25">
         <v>1</v>
       </c>
-      <c r="H34" s="20">
-        <v>10</v>
+      <c r="H34" s="20" t="s">
+        <v>31</v>
       </c>
       <c r="I34" s="20">
         <v>0</v>
@@ -8231,10 +8483,12 @@
     </row>
     <row r="35" spans="1:14" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E35" s="79">
-        <v>18</v>
+        <f>SUM(E26:E34)</f>
+        <v>21</v>
       </c>
       <c r="F35" s="79">
-        <v>19</v>
+        <f>SUM(F26:F34)</f>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -8247,7 +8501,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0460F551-2DF4-40C4-A69C-3CD7A8C42988}">
   <dimension ref="A1:I33"/>
   <sheetViews>

</xml_diff>

<commit_message>
New story tracker for Sprint 2
</commit_message>
<xml_diff>
--- a/User Story Tracker.xlsx
+++ b/User Story Tracker.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\ITGroupProject_Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\file-alpha.campus.gla.ac.uk\scsc_group2\scsc_fs_student6\student\1002243W\My Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2210F1B9-8FF8-4142-AAB6-AB255B973684}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C1D35187-1D71-4A57-A8D1-E24E8951EBBA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{12D98D7F-908C-47C5-A977-B7011EB041AE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{12D98D7F-908C-47C5-A977-B7011EB041AE}"/>
   </bookViews>
   <sheets>
     <sheet name="Timeline" sheetId="6" r:id="rId1"/>
@@ -23,8 +23,9 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Tasks Sprint 1'!$A$1:$H$21</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Tasks Sprint 2'!$A$1:$H$21</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Tasks Sprint 2'!$A$1:$I$45</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Timeline!$J$9:$N$144</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'User Stories Sprint 2'!$J$1:$K$8</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="808" uniqueCount="398">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1043" uniqueCount="476">
   <si>
     <t>User Story ID</t>
   </si>
@@ -1240,13 +1241,247 @@
   </si>
   <si>
     <t>As a user I want to be able to view aggregate statistics of past games Priority: 8 Cost 4</t>
+  </si>
+  <si>
+    <t>As a player I'd like to see statistics</t>
+  </si>
+  <si>
+    <t>As a player I'd like to start a new game</t>
+  </si>
+  <si>
+    <t>As a player I'd like to choose the number of opponents I face</t>
+  </si>
+  <si>
+    <t>As as player I'd like to see graphs/visual representation of stats (for easier understanding)</t>
+  </si>
+  <si>
+    <t>Would</t>
+  </si>
+  <si>
+    <t>As a player I'd like to quit at any time (to main menu) - not just close window</t>
+  </si>
+  <si>
+    <t>See which round I'm on</t>
+  </si>
+  <si>
+    <t>Select which attribute to use each round</t>
+  </si>
+  <si>
+    <t>See who won each round</t>
+  </si>
+  <si>
+    <t>Nice visual representation for selection/winner</t>
+  </si>
+  <si>
+    <t>Move to next round</t>
+  </si>
+  <si>
+    <t>See which attribute the opponent chose</t>
+  </si>
+  <si>
+    <t>Be able to compare winning/losing attributes after choice</t>
+  </si>
+  <si>
+    <t>See my top card (stats)</t>
+  </si>
+  <si>
+    <t>See my top card (image)</t>
+  </si>
+  <si>
+    <t>Connect to Database</t>
+  </si>
+  <si>
+    <t>Pull info from Database class</t>
+  </si>
+  <si>
+    <t>Display info</t>
+  </si>
+  <si>
+    <t>Have game data saved</t>
+  </si>
+  <si>
+    <t>Show new game button</t>
+  </si>
+  <si>
+    <t>Connect new game button to API method</t>
+  </si>
+  <si>
+    <t>Provide visual input method (dropdown?)</t>
+  </si>
+  <si>
+    <t>Pass number of players to API</t>
+  </si>
+  <si>
+    <t>Update game visuals with correct number of players</t>
+  </si>
+  <si>
+    <t>Implement some fancy javascript using database info</t>
+  </si>
+  <si>
+    <t>Learn new Javascript</t>
+  </si>
+  <si>
+    <t>Add quit button to game screen</t>
+  </si>
+  <si>
+    <t>Direct user back to menu screen (don't save stats)</t>
+  </si>
+  <si>
+    <t>Use activeCard method from game application</t>
+  </si>
+  <si>
+    <t>Pull relevant attributes into GUI (JSON?)</t>
+  </si>
+  <si>
+    <t>Prepare attributes for display(?)</t>
+  </si>
+  <si>
+    <t>Create individual spaceship images</t>
+  </si>
+  <si>
+    <t>Add images to assets folder with name -&gt; image mapping</t>
+  </si>
+  <si>
+    <t>Pull relevant image into HTML</t>
+  </si>
+  <si>
+    <t>Use getRound to pull round count</t>
+  </si>
+  <si>
+    <t>Display round in textual display</t>
+  </si>
+  <si>
+    <t>Properly display attributes (see story 6)</t>
+  </si>
+  <si>
+    <t>Be given direction on what to do next</t>
+  </si>
+  <si>
+    <t>Use GUI to select attribute (buttons?)</t>
+  </si>
+  <si>
+    <t>Send attribute selection to API for processing</t>
+  </si>
+  <si>
+    <t>Process attribute selection (user)</t>
+  </si>
+  <si>
+    <t>Process attribute of user selection (AI players)</t>
+  </si>
+  <si>
+    <t>Compare and decide winner</t>
+  </si>
+  <si>
+    <t>Display winner on GUI</t>
+  </si>
+  <si>
+    <t>Update round winner dictionary</t>
+  </si>
+  <si>
+    <t>Decide on fancy visual celebration</t>
+  </si>
+  <si>
+    <t>Add button for next round</t>
+  </si>
+  <si>
+    <t>Then display (as per story 6)</t>
+  </si>
+  <si>
+    <t>Move all player activeCards to next card (increment round count)</t>
+  </si>
+  <si>
+    <t>Process AI selection</t>
+  </si>
+  <si>
+    <t>Text output showing selection</t>
+  </si>
+  <si>
+    <t>Identify all attributes (user and AI) of selection</t>
+  </si>
+  <si>
+    <t>Highlight attribute across all users on GUI</t>
+  </si>
+  <si>
+    <t>On completion of game, write to DB</t>
+  </si>
+  <si>
+    <t>Update round messages every round</t>
+  </si>
+  <si>
+    <t>Update text for all notifications</t>
+  </si>
+  <si>
+    <t>Move to next round with user input</t>
+  </si>
+  <si>
+    <t>All on the back end</t>
+  </si>
+  <si>
+    <t>Mostly done - just pull from API and update GUI</t>
+  </si>
+  <si>
+    <t>Pull attribute names and values, update HTML</t>
+  </si>
+  <si>
+    <t>Click button, process, pass back to API</t>
+  </si>
+  <si>
+    <t>Developer story - create logging function</t>
+  </si>
+  <si>
+    <t>Developer story - testing</t>
+  </si>
+  <si>
+    <t>Developer story - code review</t>
+  </si>
+  <si>
+    <t>Output lots of strings</t>
+  </si>
+  <si>
+    <t>Create tests and implement</t>
+  </si>
+  <si>
+    <t>Review code</t>
+  </si>
+  <si>
+    <t>Responsible</t>
+  </si>
+  <si>
+    <t>Graham</t>
+  </si>
+  <si>
+    <t>Graham and Stuart</t>
+  </si>
+  <si>
+    <t>Mark and Stuart</t>
+  </si>
+  <si>
+    <t>Done (can test)</t>
+  </si>
+  <si>
+    <t>Caine</t>
+  </si>
+  <si>
+    <t>Mark</t>
+  </si>
+  <si>
+    <t>Duncan</t>
+  </si>
+  <si>
+    <t>Stuart</t>
+  </si>
+  <si>
+    <t>Sum Effort</t>
+  </si>
+  <si>
+    <t>Testing</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1277,8 +1512,37 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1327,8 +1591,29 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="31">
+  <borders count="33">
     <border>
       <left/>
       <right/>
@@ -1710,12 +1995,46 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="31" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1904,12 +2223,70 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="32" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="32" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="32" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="31" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="6">
+    <cellStyle name="20% - Accent1" xfId="5" builtinId="30"/>
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Calculation" xfId="4" builtinId="22"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="17">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -3417,18 +3794,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{45FFB758-21B8-40FE-8289-5C3EDDE78682}" name="Table1" displayName="Table1" ref="A1:I30" totalsRowShown="0" headerRowDxfId="12" headerRowBorderDxfId="11" tableBorderDxfId="10" totalsRowBorderDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{45FFB758-21B8-40FE-8289-5C3EDDE78682}" name="Table1" displayName="Table1" ref="A1:I30" totalsRowShown="0" headerRowDxfId="16" headerRowBorderDxfId="15" tableBorderDxfId="14" totalsRowBorderDxfId="13">
   <autoFilter ref="A1:I30" xr:uid="{2156CE18-A763-4159-B323-B80B9DC7677D}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{9C1C5678-4875-4C49-8346-6A8DFBEA5D13}" name="User Story ID" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{840831D9-D132-4F89-968A-D8FC7C8AE22D}" name="As a &lt;type of user&gt;" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{EFC521BE-C7AC-438B-B924-235E2C32D073}" name="I want to… &lt;perform some task&gt;" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{DCEF588C-D17D-4EFF-B0E3-050818CCF2C9}" name="… so that I can &lt;achieve some goal&gt;" dataDxfId="5"/>
-    <tableColumn id="8" xr3:uid="{B95629C5-6E7A-4C34-BBE6-E3B7097C7677}" name="Priority" dataDxfId="4"/>
-    <tableColumn id="9" xr3:uid="{4CB9E8EE-29A4-44FA-BDD7-77D58FD0D521}" name="Effort/Cost" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{5B36101A-18D1-4FB4-9EB0-DB7306ECDD34}" name="Story Complete (Y/N)" dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{C7905A7E-E306-48BA-A1D8-ACE7E65DCC03}" name="Code Complete (Feature active)" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{AD76C249-9F04-4512-AE02-18FEB1212FE9}" name="Completion Date" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{9C1C5678-4875-4C49-8346-6A8DFBEA5D13}" name="User Story ID" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{840831D9-D132-4F89-968A-D8FC7C8AE22D}" name="As a &lt;type of user&gt;" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{EFC521BE-C7AC-438B-B924-235E2C32D073}" name="I want to… &lt;perform some task&gt;" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{DCEF588C-D17D-4EFF-B0E3-050818CCF2C9}" name="… so that I can &lt;achieve some goal&gt;" dataDxfId="9"/>
+    <tableColumn id="8" xr3:uid="{B95629C5-6E7A-4C34-BBE6-E3B7097C7677}" name="Priority" dataDxfId="8"/>
+    <tableColumn id="9" xr3:uid="{4CB9E8EE-29A4-44FA-BDD7-77D58FD0D521}" name="Effort/Cost" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{5B36101A-18D1-4FB4-9EB0-DB7306ECDD34}" name="Story Complete (Y/N)" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{C7905A7E-E306-48BA-A1D8-ACE7E65DCC03}" name="Code Complete (Feature active)" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{AD76C249-9F04-4512-AE02-18FEB1212FE9}" name="Completion Date" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4355,7 +4732,7 @@
       </c>
       <c r="E25" s="54" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="F25" s="2"/>
       <c r="G25" s="61"/>
@@ -4387,7 +4764,7 @@
       </c>
       <c r="E26" s="54" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="F26" s="2"/>
       <c r="G26" s="61"/>
@@ -4419,7 +4796,7 @@
       </c>
       <c r="E27" s="54" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="F27" s="2"/>
       <c r="G27" s="61"/>
@@ -6641,7 +7018,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A10"/>
+      <selection sqref="A1:H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7348,10 +7725,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08D82316-6DF2-43BE-8926-73EBA9557747}">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7362,9 +7739,10 @@
     <col min="6" max="6" width="12.28515625" style="18" customWidth="1"/>
     <col min="7" max="7" width="27.28515625" style="18" customWidth="1"/>
     <col min="8" max="8" width="58.28515625" customWidth="1"/>
+    <col min="10" max="10" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="31" t="s">
         <v>13</v>
       </c>
@@ -7384,128 +7762,470 @@
         <v>23</v>
       </c>
       <c r="G1" s="33" t="s">
-        <v>24</v>
+        <v>465</v>
       </c>
       <c r="H1" s="34" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="27"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="28"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="22"/>
-      <c r="B3" s="29"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="21"/>
+      <c r="J1" t="s">
+        <v>465</v>
+      </c>
+      <c r="K1" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="27" t="s">
+        <v>399</v>
+      </c>
+      <c r="B2" s="29">
+        <v>2</v>
+      </c>
+      <c r="C2" s="21">
+        <v>10</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="E2" s="21">
+        <v>3</v>
+      </c>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21" t="s">
+        <v>469</v>
+      </c>
+      <c r="H2" s="23" t="s">
+        <v>456</v>
+      </c>
+      <c r="J2" t="s">
+        <v>473</v>
+      </c>
+      <c r="K2">
+        <f>SUMIF(G:G,J2,E:E)</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="22" t="s">
+        <v>411</v>
+      </c>
+      <c r="B3" s="29">
+        <v>6</v>
+      </c>
+      <c r="C3" s="21">
+        <v>9</v>
+      </c>
+      <c r="D3" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="E3" s="21">
+        <v>5</v>
+      </c>
       <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="23"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="22"/>
-      <c r="B4" s="29"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
+      <c r="G3" s="21" t="s">
+        <v>466</v>
+      </c>
+      <c r="H3" s="23" t="s">
+        <v>457</v>
+      </c>
+      <c r="J3" t="s">
+        <v>470</v>
+      </c>
+      <c r="K3">
+        <f>SUMIF(G:G,J3,E:E)</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="22" t="s">
+        <v>405</v>
+      </c>
+      <c r="B4" s="11">
+        <v>9</v>
+      </c>
+      <c r="C4" s="21">
+        <v>9</v>
+      </c>
+      <c r="D4" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="E4" s="21">
+        <v>7</v>
+      </c>
       <c r="F4" s="21"/>
-      <c r="G4" s="21"/>
-      <c r="H4" s="23"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="22"/>
-      <c r="B5" s="29"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
+      <c r="G4" s="21" t="s">
+        <v>470</v>
+      </c>
+      <c r="H4" s="23" t="s">
+        <v>458</v>
+      </c>
+      <c r="J4" t="s">
+        <v>471</v>
+      </c>
+      <c r="K4">
+        <f>SUMIF(G:G,J4,E:E)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="22" t="s">
+        <v>406</v>
+      </c>
+      <c r="B5" s="29">
+        <v>10</v>
+      </c>
+      <c r="C5" s="21">
+        <v>8</v>
+      </c>
+      <c r="D5" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="E5" s="21">
+        <v>4</v>
+      </c>
       <c r="F5" s="21"/>
-      <c r="G5" s="21"/>
+      <c r="G5" s="21" t="s">
+        <v>471</v>
+      </c>
       <c r="H5" s="23"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="22"/>
-      <c r="B6" s="29"/>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
+      <c r="J5" t="s">
+        <v>472</v>
+      </c>
+      <c r="K5">
+        <f>SUMIF(G:G,J5,E:E)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="22" t="s">
+        <v>398</v>
+      </c>
+      <c r="B6" s="29">
+        <v>1</v>
+      </c>
+      <c r="C6" s="21">
+        <v>7</v>
+      </c>
+      <c r="D6" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="E6" s="21">
+        <v>4</v>
+      </c>
       <c r="F6" s="21"/>
-      <c r="G6" s="21"/>
+      <c r="G6" s="21" t="s">
+        <v>468</v>
+      </c>
       <c r="H6" s="23"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="22"/>
-      <c r="B7" s="29"/>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
+      <c r="J6" t="s">
+        <v>469</v>
+      </c>
+      <c r="K6">
+        <f>SUMIF(G:G,J6,E:E)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="22" t="s">
+        <v>435</v>
+      </c>
+      <c r="B7" s="11">
+        <v>16</v>
+      </c>
+      <c r="C7" s="21">
+        <v>6</v>
+      </c>
+      <c r="D7" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="E7" s="21">
+        <v>3</v>
+      </c>
       <c r="F7" s="21"/>
-      <c r="G7" s="21"/>
+      <c r="G7" s="21" t="s">
+        <v>473</v>
+      </c>
       <c r="H7" s="23"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="22"/>
-      <c r="B8" s="29"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
+      <c r="J7" t="s">
+        <v>466</v>
+      </c>
+      <c r="K7">
+        <f>SUMIF(G:G,J7,E:E)</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="22" t="s">
+        <v>416</v>
+      </c>
+      <c r="B8" s="11">
+        <v>15</v>
+      </c>
+      <c r="C8" s="21">
+        <v>6</v>
+      </c>
+      <c r="D8" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="E8" s="21">
+        <v>2</v>
+      </c>
       <c r="F8" s="21"/>
-      <c r="G8" s="21"/>
-      <c r="H8" s="23"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="22"/>
-      <c r="B9" s="29"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
+      <c r="G8" s="21" t="s">
+        <v>469</v>
+      </c>
+      <c r="H8" s="23" t="s">
+        <v>455</v>
+      </c>
+      <c r="J8" t="s">
+        <v>468</v>
+      </c>
+      <c r="K8">
+        <f>SUMIF(G:G,J8,E:E)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="22" t="s">
+        <v>400</v>
+      </c>
+      <c r="B9" s="11">
+        <v>3</v>
+      </c>
+      <c r="C9" s="21">
+        <v>5</v>
+      </c>
+      <c r="D9" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="E9" s="21">
+        <v>3</v>
+      </c>
       <c r="F9" s="21"/>
-      <c r="G9" s="21"/>
+      <c r="G9" s="21" t="s">
+        <v>469</v>
+      </c>
       <c r="H9" s="23"/>
     </row>
-    <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="24"/>
-      <c r="B10" s="30"/>
-      <c r="C10" s="25"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="25"/>
-      <c r="G10" s="25"/>
-      <c r="H10" s="26"/>
+    <row r="10" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="22" t="s">
+        <v>403</v>
+      </c>
+      <c r="B10" s="29">
+        <v>5</v>
+      </c>
+      <c r="C10" s="21">
+        <v>4</v>
+      </c>
+      <c r="D10" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="E10" s="21">
+        <v>2</v>
+      </c>
+      <c r="F10" s="21"/>
+      <c r="G10" s="21" t="s">
+        <v>471</v>
+      </c>
+      <c r="H10" s="23"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="22" t="s">
+        <v>454</v>
+      </c>
+      <c r="B11" s="29">
+        <v>12</v>
+      </c>
+      <c r="C11" s="21">
+        <v>4</v>
+      </c>
+      <c r="D11" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="E11" s="21">
+        <v>4</v>
+      </c>
+      <c r="F11" s="21"/>
+      <c r="G11" s="21" t="s">
+        <v>472</v>
+      </c>
+      <c r="H11" s="23"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="22" t="s">
+        <v>404</v>
+      </c>
+      <c r="B12" s="11">
+        <v>8</v>
+      </c>
+      <c r="C12" s="21">
+        <v>3</v>
+      </c>
+      <c r="D12" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="E12" s="21">
+        <v>2</v>
+      </c>
+      <c r="F12" s="21"/>
+      <c r="G12" s="21" t="s">
+        <v>470</v>
+      </c>
+      <c r="H12" s="23"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="22" t="s">
+        <v>409</v>
+      </c>
+      <c r="B13" s="29">
+        <v>13</v>
+      </c>
+      <c r="C13" s="21">
+        <v>3</v>
+      </c>
+      <c r="D13" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="E13" s="21">
+        <v>5</v>
+      </c>
+      <c r="F13" s="21"/>
+      <c r="G13" s="21" t="s">
+        <v>470</v>
+      </c>
+      <c r="H13" s="23"/>
+    </row>
+    <row r="14" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="22" t="s">
+        <v>410</v>
+      </c>
+      <c r="B14" s="29">
+        <v>14</v>
+      </c>
+      <c r="C14" s="21">
+        <v>3</v>
+      </c>
+      <c r="D14" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="E14" s="21">
+        <v>6</v>
+      </c>
+      <c r="F14" s="21"/>
+      <c r="G14" s="21" t="s">
+        <v>471</v>
+      </c>
+      <c r="H14" s="23"/>
+    </row>
+    <row r="15" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="22" t="s">
+        <v>401</v>
+      </c>
+      <c r="B15" s="11">
+        <v>4</v>
+      </c>
+      <c r="C15" s="21">
+        <v>1</v>
+      </c>
+      <c r="D15" s="21" t="s">
+        <v>402</v>
+      </c>
+      <c r="E15" s="21">
+        <v>8</v>
+      </c>
+      <c r="F15" s="21"/>
+      <c r="G15" s="21" t="s">
+        <v>472</v>
+      </c>
+      <c r="H15" s="23"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="22" t="s">
+        <v>412</v>
+      </c>
+      <c r="B16" s="29">
+        <v>7</v>
+      </c>
+      <c r="C16" s="21">
+        <v>1</v>
+      </c>
+      <c r="D16" s="21" t="s">
+        <v>402</v>
+      </c>
+      <c r="E16" s="21">
+        <v>7</v>
+      </c>
+      <c r="F16" s="21"/>
+      <c r="G16" s="21" t="s">
+        <v>473</v>
+      </c>
+      <c r="H16" s="23"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="27" t="s">
+        <v>407</v>
+      </c>
+      <c r="B17" s="11">
+        <v>11</v>
+      </c>
+      <c r="C17" s="12">
+        <v>1</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>402</v>
+      </c>
+      <c r="E17" s="12">
+        <v>5</v>
+      </c>
+      <c r="F17" s="12"/>
+      <c r="G17" s="21" t="s">
+        <v>473</v>
+      </c>
+      <c r="H17" s="28"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="19" t="s">
+        <v>475</v>
+      </c>
+      <c r="E19" s="18">
+        <v>10</v>
+      </c>
+      <c r="G19" s="21" t="s">
+        <v>466</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="J1:K8" xr:uid="{DA8CBF8E-6484-4F4A-A5BC-0D141BE6E59E}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="J2:K8">
+      <sortCondition descending="1" ref="K1:K8"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2289136A-3240-48CC-95DE-2B454B379535}">
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E10" sqref="A10:E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.5703125" style="18" customWidth="1"/>
-    <col min="2" max="2" width="29.42578125" customWidth="1"/>
-    <col min="3" max="3" width="49.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.42578125" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" customWidth="1"/>
-    <col min="8" max="8" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="80.140625" customWidth="1"/>
+    <col min="3" max="3" width="60.28515625" customWidth="1"/>
+    <col min="4" max="4" width="17.5703125" style="18" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" style="86" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" customWidth="1"/>
+    <col min="9" max="9" width="8.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
         <v>32</v>
       </c>
@@ -7515,236 +8235,940 @@
       <c r="C1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>24</v>
+      <c r="D1" s="20" t="s">
+        <v>60</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>465</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="20"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="20">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>459</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>462</v>
+      </c>
+      <c r="D2" s="80" t="s">
+        <v>57</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>466</v>
+      </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="20"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
+      <c r="I2" s="2"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="20">
+        <v>0</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>460</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>463</v>
+      </c>
+      <c r="D3" s="80" t="s">
+        <v>57</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>467</v>
+      </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="20"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
+      <c r="I3" s="2"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="20">
+        <v>0</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>461</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>464</v>
+      </c>
+      <c r="D4" s="84" t="s">
+        <v>58</v>
+      </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="20"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
+      <c r="I4" s="2"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="20">
+        <v>1</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="D5" s="80" t="s">
+        <v>57</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>468</v>
+      </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="20"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
+      <c r="I5" s="2"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="20">
+        <v>1</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="D6" s="80" t="s">
+        <v>57</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>468</v>
+      </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="20"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
+      <c r="I6" s="2"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="20">
+        <v>1</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="D7" s="80" t="s">
+        <v>57</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>468</v>
+      </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="20"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
+      <c r="I7" s="2"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="20">
+        <v>2</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="D8" s="80" t="s">
+        <v>57</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>469</v>
+      </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="20"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
+      <c r="I8" s="2"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="20">
+        <v>2</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="D9" s="80" t="s">
+        <v>57</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>469</v>
+      </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="20"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
+      <c r="I9" s="2"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="20">
+        <v>6</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>426</v>
+      </c>
+      <c r="D10" s="80" t="s">
+        <v>57</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>466</v>
+      </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="20"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
+      <c r="I10" s="2"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="20">
+        <v>6</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="D11" s="80" t="s">
+        <v>57</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>466</v>
+      </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="20"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
+      <c r="I11" s="2"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="20">
+        <v>6</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>427</v>
+      </c>
+      <c r="D12" s="80" t="s">
+        <v>57</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>466</v>
+      </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="20"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
+      <c r="I12" s="2"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="20">
+        <v>9</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="D13" s="85" t="s">
+        <v>57</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>470</v>
+      </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="20"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
+      <c r="I13" s="2"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="20">
+        <v>9</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>436</v>
+      </c>
+      <c r="D14" s="85" t="s">
+        <v>57</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>470</v>
+      </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="20"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
+      <c r="I14" s="2"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="20">
+        <v>9</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>437</v>
+      </c>
+      <c r="D15" s="80" t="s">
+        <v>57</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>470</v>
+      </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="20"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
+      <c r="I15" s="2"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="20">
+        <v>10</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>438</v>
+      </c>
+      <c r="D16" s="80" t="s">
+        <v>57</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>471</v>
+      </c>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="20"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
+      <c r="I16" s="2"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="20">
+        <v>10</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="D17" s="80" t="s">
+        <v>57</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>471</v>
+      </c>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="20"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
+      <c r="I17" s="2"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="20">
+        <v>10</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>440</v>
+      </c>
+      <c r="D18" s="80" t="s">
+        <v>57</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>471</v>
+      </c>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="20"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
+      <c r="I18" s="2"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="20">
+        <v>10</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>441</v>
+      </c>
+      <c r="D19" s="80" t="s">
+        <v>57</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>471</v>
+      </c>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="20"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
+      <c r="I19" s="2"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="20">
+        <v>10</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>442</v>
+      </c>
+      <c r="D20" s="85" t="s">
+        <v>57</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>471</v>
+      </c>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="20"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
+      <c r="I20" s="2"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="20">
+        <v>3</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>419</v>
+      </c>
+      <c r="D21" s="84" t="s">
+        <v>58</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>469</v>
+      </c>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F22">
-        <f>SUM(F2:F21)</f>
+      <c r="I21" s="2"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="20">
+        <v>3</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>420</v>
+      </c>
+      <c r="D22" s="84" t="s">
+        <v>58</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>469</v>
+      </c>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="20">
+        <v>3</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="D23" s="81" t="s">
+        <v>58</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>469</v>
+      </c>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="20">
+        <v>4</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>401</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>423</v>
+      </c>
+      <c r="D24" s="83" t="s">
+        <v>402</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>472</v>
+      </c>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="20">
+        <v>4</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>401</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="D25" s="83" t="s">
+        <v>402</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>472</v>
+      </c>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="20">
+        <v>5</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>424</v>
+      </c>
+      <c r="D26" s="81" t="s">
+        <v>58</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>471</v>
+      </c>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="20">
+        <v>5</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>425</v>
+      </c>
+      <c r="D27" s="81" t="s">
+        <v>58</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>471</v>
+      </c>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="20">
+        <v>7</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>429</v>
+      </c>
+      <c r="D28" s="83" t="s">
+        <v>402</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>473</v>
+      </c>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="20">
+        <v>7</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="D29" s="83" t="s">
+        <v>402</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>473</v>
+      </c>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="20">
+        <v>7</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>431</v>
+      </c>
+      <c r="D30" s="83" t="s">
+        <v>402</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>473</v>
+      </c>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="20">
+        <v>8</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>404</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="D31" s="81" t="s">
+        <v>58</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>470</v>
+      </c>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="20">
+        <v>8</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>404</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="D32" s="81" t="s">
+        <v>58</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>470</v>
+      </c>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="20">
+        <v>11</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>423</v>
+      </c>
+      <c r="D33" s="82" t="s">
+        <v>402</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>473</v>
+      </c>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="2"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="20">
+        <v>11</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>443</v>
+      </c>
+      <c r="D34" s="82" t="s">
+        <v>402</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>473</v>
+      </c>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
+      <c r="I34" s="2"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="20">
+        <v>12</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="D35" s="81" t="s">
+        <v>58</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>472</v>
+      </c>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="20">
+        <v>12</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>446</v>
+      </c>
+      <c r="D36" s="81" t="s">
+        <v>58</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>472</v>
+      </c>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="2"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="20">
+        <v>12</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>445</v>
+      </c>
+      <c r="D37" s="81" t="s">
+        <v>58</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>472</v>
+      </c>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="2"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="20">
+        <v>13</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>447</v>
+      </c>
+      <c r="D38" s="81" t="s">
+        <v>58</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>470</v>
+      </c>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
+      <c r="I38" s="2"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="20">
+        <v>13</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>448</v>
+      </c>
+      <c r="D39" s="81" t="s">
+        <v>58</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>470</v>
+      </c>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
+      <c r="I39" s="2"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="20">
+        <v>14</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>449</v>
+      </c>
+      <c r="D40" s="87" t="s">
+        <v>59</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>471</v>
+      </c>
+      <c r="F40" s="2"/>
+      <c r="G40" s="2"/>
+      <c r="H40" s="2"/>
+      <c r="I40" s="2"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="20">
+        <v>14</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>450</v>
+      </c>
+      <c r="D41" s="87" t="s">
+        <v>59</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>471</v>
+      </c>
+      <c r="F41" s="2"/>
+      <c r="G41" s="2"/>
+      <c r="H41" s="2"/>
+      <c r="I41" s="2"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" s="20">
+        <v>15</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>451</v>
+      </c>
+      <c r="D42" s="81" t="s">
+        <v>58</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>469</v>
+      </c>
+      <c r="F42" s="2"/>
+      <c r="G42" s="2"/>
+      <c r="H42" s="2"/>
+      <c r="I42" s="2"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" s="20">
+        <v>16</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>435</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>452</v>
+      </c>
+      <c r="D43" s="81" t="s">
+        <v>58</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>473</v>
+      </c>
+      <c r="F43" s="2"/>
+      <c r="G43" s="2"/>
+      <c r="H43" s="2"/>
+      <c r="I43" s="2"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" s="20">
+        <v>16</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>435</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>453</v>
+      </c>
+      <c r="D44" s="81" t="s">
+        <v>58</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>473</v>
+      </c>
+      <c r="F44" s="2"/>
+      <c r="G44" s="2"/>
+      <c r="H44" s="2"/>
+      <c r="I44" s="2"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G45">
+        <f>SUM(G5:G44)</f>
         <v>0</v>
       </c>
-      <c r="G22">
-        <f>SUM(G2:G21)</f>
+      <c r="H45">
+        <f>SUM(H5:H44)</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H21" xr:uid="{9515D1DC-4AE1-4B79-A751-D444B917CA23}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H21">
-      <sortCondition ref="H1:H21"/>
+  <autoFilter ref="A1:I45" xr:uid="{9515D1DC-4AE1-4B79-A751-D444B917CA23}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I45">
+      <sortCondition sortBy="cellColor" ref="D1:D45" dxfId="3"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7755,7 +9179,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59333514-8FD2-4190-8532-38CFA6C50E52}">
   <dimension ref="A1:N35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="R18" sqref="R18"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Acceptance tests added. Red means not implemented.
</commit_message>
<xml_diff>
--- a/User Story Tracker.xlsx
+++ b/User Story Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mawhrin-Skel\eclipse-workspace\ITTeamProject_Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D25E004-13E0-4AAE-8E72-31055ED11296}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE72A707-973C-4DB8-A594-CFCB9D828B9D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" firstSheet="1" activeTab="2" xr2:uid="{12D98D7F-908C-47C5-A977-B7011EB041AE}"/>
   </bookViews>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1279" uniqueCount="556">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1280" uniqueCount="579">
   <si>
     <t>User Story ID</t>
   </si>
@@ -1530,9 +1530,6 @@
     <t>Average</t>
   </si>
   <si>
-    <t xml:space="preserve">As a human player, I want to be able to choose whether to play top trumps online or on the command line. </t>
-  </si>
-  <si>
     <t>Priority: 10 
 Effort: 2</t>
   </si>
@@ -1543,9 +1540,6 @@
     <t>User Story</t>
   </si>
   <si>
-    <t>It is complete when…</t>
-  </si>
-  <si>
     <t>Day 1</t>
   </si>
   <si>
@@ -1616,12 +1610,6 @@
 Effort: 3</t>
   </si>
   <si>
-    <t>As a human player, I want to be able to select the number of AI opponents.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  As a human player I want to have the option of starting a new game after finishing one. </t>
-  </si>
-  <si>
     <t>Priority: 8
 Effort: 1</t>
   </si>
@@ -1630,40 +1618,22 @@
 Effort: 8</t>
   </si>
   <si>
-    <t>I want to be able to view statistics concerning past games and scores.</t>
-  </si>
-  <si>
     <t>Priority: 10 
 Effort: 3</t>
   </si>
   <si>
-    <t>As a human player, I want to be able to select an attribute on my active top trumps card.</t>
-  </si>
-  <si>
-    <t>I want to be able to quit.</t>
-  </si>
-  <si>
     <t>Priority: 7
 Effort: 1</t>
   </si>
   <si>
-    <t>As a user I want to see my top card.</t>
-  </si>
-  <si>
     <t>Priority: 8
 Effort: 4</t>
   </si>
   <si>
-    <t>As a user I want to be able to view aggregate statistics of past games.</t>
-  </si>
-  <si>
     <t>Priority: 9
 Effort: 1</t>
   </si>
   <si>
-    <t>Who has won should be displayed each round.</t>
-  </si>
-  <si>
     <t>Actual Effort: 1</t>
   </si>
   <si>
@@ -1743,13 +1713,112 @@
   <si>
     <t>Priority: 1
 Effort: 5</t>
+  </si>
+  <si>
+    <t>Initiate a game via the command line or browser</t>
+  </si>
+  <si>
+    <t>As a human player, I want to be able to select the number of AI opponents</t>
+  </si>
+  <si>
+    <t>A message asks for number of players</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  As a human player I want to have the option of starting a new game after finishing one</t>
+  </si>
+  <si>
+    <t>A message asks to start a new game after finishing the last</t>
+  </si>
+  <si>
+    <t>I want to be able to view statistics concerning past games and scores</t>
+  </si>
+  <si>
+    <t>A message asks if I want to see statistics</t>
+  </si>
+  <si>
+    <t>As a human player, I want to be able to select an attribute on my active top trumps card</t>
+  </si>
+  <si>
+    <t>During the game, a message asks me to select an attribute</t>
+  </si>
+  <si>
+    <t>I want to be able to quit</t>
+  </si>
+  <si>
+    <t>A message asks if I want to quit, and exits the game if I say yes</t>
+  </si>
+  <si>
+    <t>As a user I want to see my top card</t>
+  </si>
+  <si>
+    <t>Each round I am in the game, I am shown my card details</t>
+  </si>
+  <si>
+    <t>As a user I want to be able to view aggregate statistics of past games</t>
+  </si>
+  <si>
+    <t>A message asks if I want to view statistics from past games</t>
+  </si>
+  <si>
+    <t>At the end of a round, the winners name shoud be displayed</t>
+  </si>
+  <si>
+    <t>As a human player, I want to be able to choose whether to play top trumps online or on the command line</t>
+  </si>
+  <si>
+    <t>I am shown a statistics page when I select to see it</t>
+  </si>
+  <si>
+    <t>I am shown a button to start a new game</t>
+  </si>
+  <si>
+    <t>I can see my card details on the game screen</t>
+  </si>
+  <si>
+    <t>I can click on the attribute on my card to select it</t>
+  </si>
+  <si>
+    <t>The winning player is show on the game screen</t>
+  </si>
+  <si>
+    <t>I can select the number of opponents from a drop down menu</t>
+  </si>
+  <si>
+    <t>I click a button and it takes me to the start screen</t>
+  </si>
+  <si>
+    <t>The round number is displayed on the game screen</t>
+  </si>
+  <si>
+    <t>The round counter increases when I click a new round button</t>
+  </si>
+  <si>
+    <t>A message is displayed with the attribute chosen</t>
+  </si>
+  <si>
+    <t>The game stats are saved to the database</t>
+  </si>
+  <si>
+    <t>A message is displayed with instructions</t>
+  </si>
+  <si>
+    <t>A message is displayed with all players chosen attribute</t>
+  </si>
+  <si>
+    <t>I can navigate to a page with graphs on it</t>
+  </si>
+  <si>
+    <t>I can see my top card's image on the game screen</t>
+  </si>
+  <si>
+    <t>Who won is displayed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1825,6 +1894,13 @@
     <font>
       <sz val="16"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2460,7 +2536,7 @@
     <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="153">
+  <cellXfs count="154">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -2838,6 +2914,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -12663,8 +12742,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C084741F-CB12-4A6B-96B9-249D88E345EF}">
   <dimension ref="A1:AA383"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A160" workbookViewId="0">
-      <selection activeCell="V375" sqref="V375:Z382"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AC16" sqref="AC16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12704,7 +12783,7 @@
     <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" s="39"/>
       <c r="B2" s="132" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="C2" s="133"/>
       <c r="D2" s="133"/>
@@ -12719,7 +12798,7 @@
       <c r="M2" s="128"/>
       <c r="O2" s="39"/>
       <c r="P2" s="132" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="Q2" s="133"/>
       <c r="R2" s="133"/>
@@ -12764,7 +12843,7 @@
     <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" s="39"/>
       <c r="B4" s="138" t="s">
-        <v>492</v>
+        <v>562</v>
       </c>
       <c r="C4" s="139"/>
       <c r="D4" s="139"/>
@@ -12772,7 +12851,7 @@
       <c r="F4" s="139"/>
       <c r="G4" s="139"/>
       <c r="H4" s="139" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="I4" s="144"/>
       <c r="J4" s="144"/>
@@ -12789,7 +12868,7 @@
       <c r="T4" s="139"/>
       <c r="U4" s="139"/>
       <c r="V4" s="139" t="s">
-        <v>539</v>
+        <v>529</v>
       </c>
       <c r="W4" s="144"/>
       <c r="X4" s="144"/>
@@ -13024,7 +13103,7 @@
     <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" s="39"/>
       <c r="B13" s="132" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C13" s="133"/>
       <c r="D13" s="133"/>
@@ -13039,7 +13118,7 @@
       <c r="M13" s="128"/>
       <c r="O13" s="39"/>
       <c r="P13" s="132" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="Q13" s="133"/>
       <c r="R13" s="133"/>
@@ -13084,7 +13163,7 @@
     <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15" s="39"/>
       <c r="B15" s="150" t="s">
-        <v>496</v>
+        <v>546</v>
       </c>
       <c r="C15" s="144"/>
       <c r="D15" s="144"/>
@@ -13092,7 +13171,7 @@
       <c r="F15" s="144"/>
       <c r="G15" s="144"/>
       <c r="H15" s="144" t="s">
-        <v>534</v>
+        <v>524</v>
       </c>
       <c r="I15" s="144"/>
       <c r="J15" s="144"/>
@@ -13101,7 +13180,7 @@
       <c r="M15" s="128"/>
       <c r="O15" s="39"/>
       <c r="P15" s="150" t="s">
-        <v>496</v>
+        <v>563</v>
       </c>
       <c r="Q15" s="144"/>
       <c r="R15" s="144"/>
@@ -13109,7 +13188,7 @@
       <c r="T15" s="144"/>
       <c r="U15" s="144"/>
       <c r="V15" s="144" t="s">
-        <v>540</v>
+        <v>530</v>
       </c>
       <c r="W15" s="144"/>
       <c r="X15" s="144"/>
@@ -13373,7 +13452,7 @@
     <row r="26" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A26" s="39"/>
       <c r="B26" s="132" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="C26" s="133"/>
       <c r="D26" s="133"/>
@@ -13388,7 +13467,7 @@
       <c r="M26" s="128"/>
       <c r="O26" s="39"/>
       <c r="P26" s="132" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="Q26" s="133"/>
       <c r="R26" s="133"/>
@@ -13433,7 +13512,7 @@
     <row r="28" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A28" s="39"/>
       <c r="B28" s="138" t="s">
-        <v>520</v>
+        <v>547</v>
       </c>
       <c r="C28" s="139"/>
       <c r="D28" s="139"/>
@@ -13441,7 +13520,7 @@
       <c r="F28" s="139"/>
       <c r="G28" s="139"/>
       <c r="H28" s="139" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="I28" s="144"/>
       <c r="J28" s="144"/>
@@ -13458,7 +13537,7 @@
       <c r="T28" s="139"/>
       <c r="U28" s="139"/>
       <c r="V28" s="139" t="s">
-        <v>525</v>
+        <v>520</v>
       </c>
       <c r="W28" s="144"/>
       <c r="X28" s="144"/>
@@ -13693,7 +13772,7 @@
     <row r="37" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A37" s="39"/>
       <c r="B37" s="132" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C37" s="133"/>
       <c r="D37" s="133"/>
@@ -13708,7 +13787,7 @@
       <c r="M37" s="128"/>
       <c r="O37" s="39"/>
       <c r="P37" s="132" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="Q37" s="133"/>
       <c r="R37" s="133"/>
@@ -13752,14 +13831,16 @@
     </row>
     <row r="39" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A39" s="39"/>
-      <c r="B39" s="150"/>
+      <c r="B39" s="150" t="s">
+        <v>548</v>
+      </c>
       <c r="C39" s="144"/>
       <c r="D39" s="144"/>
       <c r="E39" s="144"/>
       <c r="F39" s="144"/>
       <c r="G39" s="144"/>
       <c r="H39" s="144" t="s">
-        <v>535</v>
+        <v>525</v>
       </c>
       <c r="I39" s="144"/>
       <c r="J39" s="144"/>
@@ -13768,7 +13849,7 @@
       <c r="M39" s="128"/>
       <c r="O39" s="39"/>
       <c r="P39" s="150" t="s">
-        <v>496</v>
+        <v>564</v>
       </c>
       <c r="Q39" s="144"/>
       <c r="R39" s="144"/>
@@ -13776,7 +13857,7 @@
       <c r="T39" s="144"/>
       <c r="U39" s="144"/>
       <c r="V39" s="144" t="s">
-        <v>536</v>
+        <v>526</v>
       </c>
       <c r="W39" s="144"/>
       <c r="X39" s="144"/>
@@ -14040,7 +14121,7 @@
     <row r="50" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A50" s="39"/>
       <c r="B50" s="132" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="C50" s="133"/>
       <c r="D50" s="133"/>
@@ -14055,7 +14136,7 @@
       <c r="M50" s="128"/>
       <c r="O50" s="39"/>
       <c r="P50" s="132" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="Q50" s="133"/>
       <c r="R50" s="133"/>
@@ -14100,7 +14181,7 @@
     <row r="52" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A52" s="39"/>
       <c r="B52" s="138" t="s">
-        <v>521</v>
+        <v>549</v>
       </c>
       <c r="C52" s="139"/>
       <c r="D52" s="139"/>
@@ -14108,7 +14189,7 @@
       <c r="F52" s="139"/>
       <c r="G52" s="139"/>
       <c r="H52" s="139" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
       <c r="I52" s="144"/>
       <c r="J52" s="144"/>
@@ -14125,7 +14206,7 @@
       <c r="T52" s="139"/>
       <c r="U52" s="139"/>
       <c r="V52" s="139" t="s">
-        <v>541</v>
+        <v>531</v>
       </c>
       <c r="W52" s="144"/>
       <c r="X52" s="144"/>
@@ -14360,7 +14441,7 @@
     <row r="61" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A61" s="39"/>
       <c r="B61" s="132" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C61" s="133"/>
       <c r="D61" s="133"/>
@@ -14375,7 +14456,7 @@
       <c r="M61" s="128"/>
       <c r="O61" s="39"/>
       <c r="P61" s="132" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="Q61" s="133"/>
       <c r="R61" s="133"/>
@@ -14420,7 +14501,7 @@
     <row r="63" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A63" s="39"/>
       <c r="B63" s="150" t="s">
-        <v>496</v>
+        <v>550</v>
       </c>
       <c r="C63" s="144"/>
       <c r="D63" s="144"/>
@@ -14428,7 +14509,7 @@
       <c r="F63" s="144"/>
       <c r="G63" s="144"/>
       <c r="H63" s="144" t="s">
-        <v>536</v>
+        <v>526</v>
       </c>
       <c r="I63" s="144"/>
       <c r="J63" s="144"/>
@@ -14437,7 +14518,7 @@
       <c r="M63" s="128"/>
       <c r="O63" s="39"/>
       <c r="P63" s="150" t="s">
-        <v>496</v>
+        <v>565</v>
       </c>
       <c r="Q63" s="144"/>
       <c r="R63" s="144"/>
@@ -14445,7 +14526,7 @@
       <c r="T63" s="144"/>
       <c r="U63" s="144"/>
       <c r="V63" s="144" t="s">
-        <v>542</v>
+        <v>532</v>
       </c>
       <c r="W63" s="144"/>
       <c r="X63" s="144"/>
@@ -14709,7 +14790,7 @@
     <row r="74" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A74" s="39"/>
       <c r="B74" s="132" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="C74" s="133"/>
       <c r="D74" s="133"/>
@@ -14724,7 +14805,7 @@
       <c r="M74" s="128"/>
       <c r="O74" s="39"/>
       <c r="P74" s="132" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="Q74" s="133"/>
       <c r="R74" s="133"/>
@@ -14769,7 +14850,7 @@
     <row r="76" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A76" s="39"/>
       <c r="B76" s="138" t="s">
-        <v>524</v>
+        <v>551</v>
       </c>
       <c r="C76" s="139"/>
       <c r="D76" s="139"/>
@@ -14777,7 +14858,7 @@
       <c r="F76" s="139"/>
       <c r="G76" s="139"/>
       <c r="H76" s="139" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
       <c r="I76" s="144"/>
       <c r="J76" s="144"/>
@@ -14794,7 +14875,7 @@
       <c r="T76" s="139"/>
       <c r="U76" s="139"/>
       <c r="V76" s="139" t="s">
-        <v>543</v>
+        <v>533</v>
       </c>
       <c r="W76" s="144"/>
       <c r="X76" s="144"/>
@@ -15029,7 +15110,7 @@
     <row r="85" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A85" s="39"/>
       <c r="B85" s="132" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C85" s="133"/>
       <c r="D85" s="133"/>
@@ -15044,7 +15125,7 @@
       <c r="M85" s="128"/>
       <c r="O85" s="39"/>
       <c r="P85" s="132" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="Q85" s="133"/>
       <c r="R85" s="133"/>
@@ -15089,7 +15170,7 @@
     <row r="87" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A87" s="39"/>
       <c r="B87" s="150" t="s">
-        <v>496</v>
+        <v>552</v>
       </c>
       <c r="C87" s="144"/>
       <c r="D87" s="144"/>
@@ -15097,7 +15178,7 @@
       <c r="F87" s="144"/>
       <c r="G87" s="144"/>
       <c r="H87" s="144" t="s">
-        <v>537</v>
+        <v>527</v>
       </c>
       <c r="I87" s="144"/>
       <c r="J87" s="144"/>
@@ -15106,7 +15187,7 @@
       <c r="M87" s="128"/>
       <c r="O87" s="39"/>
       <c r="P87" s="150" t="s">
-        <v>496</v>
+        <v>566</v>
       </c>
       <c r="Q87" s="144"/>
       <c r="R87" s="144"/>
@@ -15114,7 +15195,7 @@
       <c r="T87" s="144"/>
       <c r="U87" s="144"/>
       <c r="V87" s="144" t="s">
-        <v>537</v>
+        <v>527</v>
       </c>
       <c r="W87" s="144"/>
       <c r="X87" s="144"/>
@@ -15378,7 +15459,7 @@
     <row r="98" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A98" s="39"/>
       <c r="B98" s="132" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="C98" s="133"/>
       <c r="D98" s="133"/>
@@ -15393,7 +15474,7 @@
       <c r="M98" s="128"/>
       <c r="O98" s="39"/>
       <c r="P98" s="132" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="Q98" s="133"/>
       <c r="R98" s="133"/>
@@ -15438,7 +15519,7 @@
     <row r="100" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A100" s="39"/>
       <c r="B100" s="138" t="s">
-        <v>526</v>
+        <v>553</v>
       </c>
       <c r="C100" s="139"/>
       <c r="D100" s="139"/>
@@ -15446,7 +15527,7 @@
       <c r="F100" s="139"/>
       <c r="G100" s="139"/>
       <c r="H100" s="139" t="s">
-        <v>525</v>
+        <v>520</v>
       </c>
       <c r="I100" s="144"/>
       <c r="J100" s="144"/>
@@ -15463,7 +15544,7 @@
       <c r="T100" s="139"/>
       <c r="U100" s="139"/>
       <c r="V100" s="139" t="s">
-        <v>544</v>
+        <v>534</v>
       </c>
       <c r="W100" s="144"/>
       <c r="X100" s="144"/>
@@ -15698,7 +15779,7 @@
     <row r="109" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A109" s="39"/>
       <c r="B109" s="132" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C109" s="133"/>
       <c r="D109" s="133"/>
@@ -15713,7 +15794,7 @@
       <c r="M109" s="128"/>
       <c r="O109" s="39"/>
       <c r="P109" s="132" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="Q109" s="133"/>
       <c r="R109" s="133"/>
@@ -15758,7 +15839,7 @@
     <row r="111" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A111" s="39"/>
       <c r="B111" s="150" t="s">
-        <v>496</v>
+        <v>554</v>
       </c>
       <c r="C111" s="144"/>
       <c r="D111" s="144"/>
@@ -15766,7 +15847,7 @@
       <c r="F111" s="144"/>
       <c r="G111" s="144"/>
       <c r="H111" s="144" t="s">
-        <v>536</v>
+        <v>526</v>
       </c>
       <c r="I111" s="144"/>
       <c r="J111" s="144"/>
@@ -15775,7 +15856,7 @@
       <c r="M111" s="128"/>
       <c r="O111" s="39"/>
       <c r="P111" s="150" t="s">
-        <v>496</v>
+        <v>567</v>
       </c>
       <c r="Q111" s="144"/>
       <c r="R111" s="144"/>
@@ -15783,7 +15864,7 @@
       <c r="T111" s="144"/>
       <c r="U111" s="144"/>
       <c r="V111" s="144" t="s">
-        <v>536</v>
+        <v>526</v>
       </c>
       <c r="W111" s="144"/>
       <c r="X111" s="144"/>
@@ -16047,7 +16128,7 @@
     <row r="122" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A122" s="39"/>
       <c r="B122" s="132" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="C122" s="133"/>
       <c r="D122" s="133"/>
@@ -16062,7 +16143,7 @@
       <c r="M122" s="128"/>
       <c r="O122" s="39"/>
       <c r="P122" s="132" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="Q122" s="133"/>
       <c r="R122" s="133"/>
@@ -16107,7 +16188,7 @@
     <row r="124" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A124" s="39"/>
       <c r="B124" s="138" t="s">
-        <v>527</v>
+        <v>555</v>
       </c>
       <c r="C124" s="139"/>
       <c r="D124" s="139"/>
@@ -16115,7 +16196,7 @@
       <c r="F124" s="139"/>
       <c r="G124" s="139"/>
       <c r="H124" s="139" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
       <c r="I124" s="144"/>
       <c r="J124" s="144"/>
@@ -16132,7 +16213,7 @@
       <c r="T124" s="139"/>
       <c r="U124" s="139"/>
       <c r="V124" s="139" t="s">
-        <v>545</v>
+        <v>535</v>
       </c>
       <c r="W124" s="144"/>
       <c r="X124" s="144"/>
@@ -16367,7 +16448,7 @@
     <row r="133" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A133" s="39"/>
       <c r="B133" s="132" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C133" s="133"/>
       <c r="D133" s="133"/>
@@ -16382,7 +16463,7 @@
       <c r="M133" s="128"/>
       <c r="O133" s="39"/>
       <c r="P133" s="132" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="Q133" s="133"/>
       <c r="R133" s="133"/>
@@ -16427,7 +16508,7 @@
     <row r="135" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A135" s="39"/>
       <c r="B135" s="150" t="s">
-        <v>496</v>
+        <v>556</v>
       </c>
       <c r="C135" s="144"/>
       <c r="D135" s="144"/>
@@ -16435,7 +16516,7 @@
       <c r="F135" s="144"/>
       <c r="G135" s="144"/>
       <c r="H135" s="144" t="s">
-        <v>535</v>
+        <v>525</v>
       </c>
       <c r="I135" s="144"/>
       <c r="J135" s="144"/>
@@ -16444,7 +16525,7 @@
       <c r="M135" s="128"/>
       <c r="O135" s="39"/>
       <c r="P135" s="150" t="s">
-        <v>496</v>
+        <v>568</v>
       </c>
       <c r="Q135" s="144"/>
       <c r="R135" s="144"/>
@@ -16452,7 +16533,7 @@
       <c r="T135" s="144"/>
       <c r="U135" s="144"/>
       <c r="V135" s="144" t="s">
-        <v>535</v>
+        <v>525</v>
       </c>
       <c r="W135" s="144"/>
       <c r="X135" s="144"/>
@@ -16716,7 +16797,7 @@
     <row r="146" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A146" s="39"/>
       <c r="B146" s="132" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="C146" s="133"/>
       <c r="D146" s="133"/>
@@ -16731,7 +16812,7 @@
       <c r="M146" s="128"/>
       <c r="O146" s="39"/>
       <c r="P146" s="132" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="Q146" s="133"/>
       <c r="R146" s="133"/>
@@ -16776,7 +16857,7 @@
     <row r="148" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A148" s="39"/>
       <c r="B148" s="138" t="s">
-        <v>529</v>
+        <v>557</v>
       </c>
       <c r="C148" s="139"/>
       <c r="D148" s="139"/>
@@ -16784,7 +16865,7 @@
       <c r="F148" s="139"/>
       <c r="G148" s="139"/>
       <c r="H148" s="139" t="s">
-        <v>528</v>
+        <v>521</v>
       </c>
       <c r="I148" s="144"/>
       <c r="J148" s="144"/>
@@ -16801,7 +16882,7 @@
       <c r="T148" s="139"/>
       <c r="U148" s="139"/>
       <c r="V148" s="139" t="s">
-        <v>546</v>
+        <v>536</v>
       </c>
       <c r="W148" s="144"/>
       <c r="X148" s="144"/>
@@ -17036,7 +17117,7 @@
     <row r="157" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A157" s="39"/>
       <c r="B157" s="132" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C157" s="133"/>
       <c r="D157" s="133"/>
@@ -17051,7 +17132,7 @@
       <c r="M157" s="128"/>
       <c r="O157" s="39"/>
       <c r="P157" s="132" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="Q157" s="133"/>
       <c r="R157" s="133"/>
@@ -17096,7 +17177,7 @@
     <row r="159" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A159" s="39"/>
       <c r="B159" s="150" t="s">
-        <v>496</v>
+        <v>558</v>
       </c>
       <c r="C159" s="144"/>
       <c r="D159" s="144"/>
@@ -17104,7 +17185,7 @@
       <c r="F159" s="144"/>
       <c r="G159" s="144"/>
       <c r="H159" s="144" t="s">
-        <v>535</v>
+        <v>525</v>
       </c>
       <c r="I159" s="144"/>
       <c r="J159" s="144"/>
@@ -17113,7 +17194,7 @@
       <c r="M159" s="128"/>
       <c r="O159" s="39"/>
       <c r="P159" s="150" t="s">
-        <v>496</v>
+        <v>569</v>
       </c>
       <c r="Q159" s="144"/>
       <c r="R159" s="144"/>
@@ -17121,7 +17202,7 @@
       <c r="T159" s="144"/>
       <c r="U159" s="144"/>
       <c r="V159" s="144" t="s">
-        <v>542</v>
+        <v>532</v>
       </c>
       <c r="W159" s="144"/>
       <c r="X159" s="144"/>
@@ -17385,7 +17466,7 @@
     <row r="170" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A170" s="39"/>
       <c r="B170" s="132" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="C170" s="133"/>
       <c r="D170" s="133"/>
@@ -17400,7 +17481,7 @@
       <c r="M170" s="128"/>
       <c r="O170" s="39"/>
       <c r="P170" s="132" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="Q170" s="133"/>
       <c r="R170" s="133"/>
@@ -17445,7 +17526,7 @@
     <row r="172" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A172" s="39"/>
       <c r="B172" s="138" t="s">
-        <v>531</v>
+        <v>559</v>
       </c>
       <c r="C172" s="139"/>
       <c r="D172" s="139"/>
@@ -17453,7 +17534,7 @@
       <c r="F172" s="139"/>
       <c r="G172" s="139"/>
       <c r="H172" s="139" t="s">
-        <v>530</v>
+        <v>522</v>
       </c>
       <c r="I172" s="144"/>
       <c r="J172" s="144"/>
@@ -17470,7 +17551,7 @@
       <c r="T172" s="139"/>
       <c r="U172" s="139"/>
       <c r="V172" s="139" t="s">
-        <v>547</v>
+        <v>537</v>
       </c>
       <c r="W172" s="144"/>
       <c r="X172" s="144"/>
@@ -17705,7 +17786,7 @@
     <row r="181" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A181" s="39"/>
       <c r="B181" s="132" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C181" s="133"/>
       <c r="D181" s="133"/>
@@ -17720,7 +17801,7 @@
       <c r="M181" s="128"/>
       <c r="O181" s="39"/>
       <c r="P181" s="132" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="Q181" s="133"/>
       <c r="R181" s="133"/>
@@ -17765,7 +17846,7 @@
     <row r="183" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A183" s="39"/>
       <c r="B183" s="150" t="s">
-        <v>496</v>
+        <v>560</v>
       </c>
       <c r="C183" s="144"/>
       <c r="D183" s="144"/>
@@ -17773,7 +17854,7 @@
       <c r="F183" s="144"/>
       <c r="G183" s="144"/>
       <c r="H183" s="144" t="s">
-        <v>538</v>
+        <v>528</v>
       </c>
       <c r="I183" s="144"/>
       <c r="J183" s="144"/>
@@ -17782,7 +17863,7 @@
       <c r="M183" s="128"/>
       <c r="O183" s="39"/>
       <c r="P183" s="150" t="s">
-        <v>496</v>
+        <v>570</v>
       </c>
       <c r="Q183" s="144"/>
       <c r="R183" s="144"/>
@@ -17790,7 +17871,7 @@
       <c r="T183" s="144"/>
       <c r="U183" s="144"/>
       <c r="V183" s="144" t="s">
-        <v>536</v>
+        <v>526</v>
       </c>
       <c r="W183" s="144"/>
       <c r="X183" s="144"/>
@@ -18054,7 +18135,7 @@
     <row r="194" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A194" s="39"/>
       <c r="B194" s="132" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="C194" s="133"/>
       <c r="D194" s="133"/>
@@ -18069,7 +18150,7 @@
       <c r="M194" s="128"/>
       <c r="O194" s="39"/>
       <c r="P194" s="132" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="Q194" s="133"/>
       <c r="R194" s="133"/>
@@ -18114,7 +18195,7 @@
     <row r="196" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A196" s="39"/>
       <c r="B196" s="138" t="s">
-        <v>533</v>
+        <v>389</v>
       </c>
       <c r="C196" s="139"/>
       <c r="D196" s="139"/>
@@ -18122,7 +18203,7 @@
       <c r="F196" s="139"/>
       <c r="G196" s="139"/>
       <c r="H196" s="139" t="s">
-        <v>532</v>
+        <v>523</v>
       </c>
       <c r="I196" s="144"/>
       <c r="J196" s="144"/>
@@ -18139,7 +18220,7 @@
       <c r="T196" s="139"/>
       <c r="U196" s="139"/>
       <c r="V196" s="139" t="s">
-        <v>549</v>
+        <v>539</v>
       </c>
       <c r="W196" s="144"/>
       <c r="X196" s="144"/>
@@ -18374,7 +18455,7 @@
     <row r="205" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A205" s="39"/>
       <c r="B205" s="132" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C205" s="133"/>
       <c r="D205" s="133"/>
@@ -18389,7 +18470,7 @@
       <c r="M205" s="128"/>
       <c r="O205" s="39"/>
       <c r="P205" s="132" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="Q205" s="133"/>
       <c r="R205" s="133"/>
@@ -18434,7 +18515,7 @@
     <row r="207" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A207" s="39"/>
       <c r="B207" s="150" t="s">
-        <v>496</v>
+        <v>561</v>
       </c>
       <c r="C207" s="144"/>
       <c r="D207" s="144"/>
@@ -18442,7 +18523,7 @@
       <c r="F207" s="144"/>
       <c r="G207" s="144"/>
       <c r="H207" s="144" t="s">
-        <v>534</v>
+        <v>524</v>
       </c>
       <c r="I207" s="144"/>
       <c r="J207" s="144"/>
@@ -18451,7 +18532,7 @@
       <c r="M207" s="128"/>
       <c r="O207" s="39"/>
       <c r="P207" s="150" t="s">
-        <v>496</v>
+        <v>571</v>
       </c>
       <c r="Q207" s="144"/>
       <c r="R207" s="144"/>
@@ -18459,7 +18540,7 @@
       <c r="T207" s="144"/>
       <c r="U207" s="144"/>
       <c r="V207" s="144" t="s">
-        <v>538</v>
+        <v>528</v>
       </c>
       <c r="W207" s="144"/>
       <c r="X207" s="144"/>
@@ -18710,7 +18791,7 @@
     <row r="218" spans="1:27" x14ac:dyDescent="0.25">
       <c r="O218" s="39"/>
       <c r="P218" s="132" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="Q218" s="133"/>
       <c r="R218" s="133"/>
@@ -18750,7 +18831,7 @@
       <c r="T220" s="139"/>
       <c r="U220" s="139"/>
       <c r="V220" s="139" t="s">
-        <v>548</v>
+        <v>538</v>
       </c>
       <c r="W220" s="144"/>
       <c r="X220" s="144"/>
@@ -18881,7 +18962,7 @@
     <row r="229" spans="15:27" x14ac:dyDescent="0.25">
       <c r="O229" s="39"/>
       <c r="P229" s="132" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="Q229" s="133"/>
       <c r="R229" s="133"/>
@@ -18913,7 +18994,7 @@
     <row r="231" spans="15:27" x14ac:dyDescent="0.25">
       <c r="O231" s="39"/>
       <c r="P231" s="150" t="s">
-        <v>496</v>
+        <v>572</v>
       </c>
       <c r="Q231" s="144"/>
       <c r="R231" s="144"/>
@@ -18921,7 +19002,7 @@
       <c r="T231" s="144"/>
       <c r="U231" s="144"/>
       <c r="V231" s="144" t="s">
-        <v>536</v>
+        <v>526</v>
       </c>
       <c r="W231" s="144"/>
       <c r="X231" s="144"/>
@@ -19068,7 +19149,7 @@
     <row r="242" spans="15:27" x14ac:dyDescent="0.25">
       <c r="O242" s="39"/>
       <c r="P242" s="132" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="Q242" s="133"/>
       <c r="R242" s="133"/>
@@ -19108,7 +19189,7 @@
       <c r="T244" s="139"/>
       <c r="U244" s="139"/>
       <c r="V244" s="139" t="s">
-        <v>550</v>
+        <v>540</v>
       </c>
       <c r="W244" s="144"/>
       <c r="X244" s="144"/>
@@ -19239,7 +19320,7 @@
     <row r="253" spans="15:27" x14ac:dyDescent="0.25">
       <c r="O253" s="39"/>
       <c r="P253" s="132" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="Q253" s="133"/>
       <c r="R253" s="133"/>
@@ -19271,7 +19352,7 @@
     <row r="255" spans="15:27" x14ac:dyDescent="0.25">
       <c r="O255" s="39"/>
       <c r="P255" s="150" t="s">
-        <v>496</v>
+        <v>573</v>
       </c>
       <c r="Q255" s="144"/>
       <c r="R255" s="144"/>
@@ -19279,7 +19360,7 @@
       <c r="T255" s="144"/>
       <c r="U255" s="144"/>
       <c r="V255" s="144" t="s">
-        <v>535</v>
+        <v>525</v>
       </c>
       <c r="W255" s="144"/>
       <c r="X255" s="144"/>
@@ -19426,7 +19507,7 @@
     <row r="266" spans="15:27" x14ac:dyDescent="0.25">
       <c r="O266" s="39"/>
       <c r="P266" s="132" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="Q266" s="133"/>
       <c r="R266" s="133"/>
@@ -19466,7 +19547,7 @@
       <c r="T268" s="139"/>
       <c r="U268" s="139"/>
       <c r="V268" s="139" t="s">
-        <v>551</v>
+        <v>541</v>
       </c>
       <c r="W268" s="144"/>
       <c r="X268" s="144"/>
@@ -19597,7 +19678,7 @@
     <row r="277" spans="15:27" x14ac:dyDescent="0.25">
       <c r="O277" s="39"/>
       <c r="P277" s="132" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="Q277" s="133"/>
       <c r="R277" s="133"/>
@@ -19629,7 +19710,7 @@
     <row r="279" spans="15:27" x14ac:dyDescent="0.25">
       <c r="O279" s="39"/>
       <c r="P279" s="150" t="s">
-        <v>496</v>
+        <v>574</v>
       </c>
       <c r="Q279" s="144"/>
       <c r="R279" s="144"/>
@@ -19637,7 +19718,7 @@
       <c r="T279" s="144"/>
       <c r="U279" s="144"/>
       <c r="V279" s="144" t="s">
-        <v>536</v>
+        <v>526</v>
       </c>
       <c r="W279" s="144"/>
       <c r="X279" s="144"/>
@@ -19784,7 +19865,7 @@
     <row r="290" spans="15:27" x14ac:dyDescent="0.25">
       <c r="O290" s="39"/>
       <c r="P290" s="132" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="Q290" s="133"/>
       <c r="R290" s="133"/>
@@ -19824,7 +19905,7 @@
       <c r="T292" s="139"/>
       <c r="U292" s="139"/>
       <c r="V292" s="139" t="s">
-        <v>552</v>
+        <v>542</v>
       </c>
       <c r="W292" s="144"/>
       <c r="X292" s="144"/>
@@ -19955,7 +20036,7 @@
     <row r="301" spans="15:27" x14ac:dyDescent="0.25">
       <c r="O301" s="39"/>
       <c r="P301" s="132" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="Q301" s="133"/>
       <c r="R301" s="133"/>
@@ -19986,8 +20067,8 @@
     </row>
     <row r="303" spans="15:27" x14ac:dyDescent="0.25">
       <c r="O303" s="39"/>
-      <c r="P303" s="150" t="s">
-        <v>496</v>
+      <c r="P303" s="153" t="s">
+        <v>575</v>
       </c>
       <c r="Q303" s="144"/>
       <c r="R303" s="144"/>
@@ -19995,7 +20076,7 @@
       <c r="T303" s="144"/>
       <c r="U303" s="144"/>
       <c r="V303" s="144" t="s">
-        <v>537</v>
+        <v>527</v>
       </c>
       <c r="W303" s="144"/>
       <c r="X303" s="144"/>
@@ -20142,7 +20223,7 @@
     <row r="314" spans="15:27" x14ac:dyDescent="0.25">
       <c r="O314" s="39"/>
       <c r="P314" s="132" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="Q314" s="133"/>
       <c r="R314" s="133"/>
@@ -20182,7 +20263,7 @@
       <c r="T316" s="139"/>
       <c r="U316" s="139"/>
       <c r="V316" s="139" t="s">
-        <v>553</v>
+        <v>543</v>
       </c>
       <c r="W316" s="144"/>
       <c r="X316" s="144"/>
@@ -20313,7 +20394,7 @@
     <row r="325" spans="15:27" x14ac:dyDescent="0.25">
       <c r="O325" s="39"/>
       <c r="P325" s="132" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="Q325" s="133"/>
       <c r="R325" s="133"/>
@@ -20345,7 +20426,7 @@
     <row r="327" spans="15:27" x14ac:dyDescent="0.25">
       <c r="O327" s="39"/>
       <c r="P327" s="150" t="s">
-        <v>496</v>
+        <v>576</v>
       </c>
       <c r="Q327" s="144"/>
       <c r="R327" s="144"/>
@@ -20353,7 +20434,7 @@
       <c r="T327" s="144"/>
       <c r="U327" s="144"/>
       <c r="V327" s="144" t="s">
-        <v>542</v>
+        <v>532</v>
       </c>
       <c r="W327" s="144"/>
       <c r="X327" s="144"/>
@@ -20500,7 +20581,7 @@
     <row r="338" spans="15:27" x14ac:dyDescent="0.25">
       <c r="O338" s="39"/>
       <c r="P338" s="132" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="Q338" s="133"/>
       <c r="R338" s="133"/>
@@ -20540,7 +20621,7 @@
       <c r="T340" s="139"/>
       <c r="U340" s="139"/>
       <c r="V340" s="139" t="s">
-        <v>554</v>
+        <v>544</v>
       </c>
       <c r="W340" s="144"/>
       <c r="X340" s="144"/>
@@ -20671,7 +20752,7 @@
     <row r="349" spans="15:27" x14ac:dyDescent="0.25">
       <c r="O349" s="39"/>
       <c r="P349" s="132" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="Q349" s="133"/>
       <c r="R349" s="133"/>
@@ -20703,7 +20784,7 @@
     <row r="351" spans="15:27" x14ac:dyDescent="0.25">
       <c r="O351" s="39"/>
       <c r="P351" s="150" t="s">
-        <v>496</v>
+        <v>577</v>
       </c>
       <c r="Q351" s="144"/>
       <c r="R351" s="144"/>
@@ -20711,7 +20792,7 @@
       <c r="T351" s="144"/>
       <c r="U351" s="144"/>
       <c r="V351" s="144" t="s">
-        <v>538</v>
+        <v>528</v>
       </c>
       <c r="W351" s="144"/>
       <c r="X351" s="144"/>
@@ -20858,7 +20939,7 @@
     <row r="362" spans="15:27" x14ac:dyDescent="0.25">
       <c r="O362" s="39"/>
       <c r="P362" s="132" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="Q362" s="133"/>
       <c r="R362" s="133"/>
@@ -20898,7 +20979,7 @@
       <c r="T364" s="139"/>
       <c r="U364" s="139"/>
       <c r="V364" s="139" t="s">
-        <v>555</v>
+        <v>545</v>
       </c>
       <c r="W364" s="144"/>
       <c r="X364" s="144"/>
@@ -21029,7 +21110,7 @@
     <row r="373" spans="15:27" x14ac:dyDescent="0.25">
       <c r="O373" s="39"/>
       <c r="P373" s="132" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="Q373" s="133"/>
       <c r="R373" s="133"/>
@@ -21060,8 +21141,8 @@
     </row>
     <row r="375" spans="15:27" x14ac:dyDescent="0.25">
       <c r="O375" s="39"/>
-      <c r="P375" s="150" t="s">
-        <v>496</v>
+      <c r="P375" s="153" t="s">
+        <v>578</v>
       </c>
       <c r="Q375" s="144"/>
       <c r="R375" s="144"/>
@@ -21069,7 +21150,7 @@
       <c r="T375" s="144"/>
       <c r="U375" s="144"/>
       <c r="V375" s="144" t="s">
-        <v>540</v>
+        <v>530</v>
       </c>
       <c r="W375" s="144"/>
       <c r="X375" s="144"/>
@@ -21199,6 +21280,144 @@
     </row>
   </sheetData>
   <mergeCells count="150">
+    <mergeCell ref="B2:L3"/>
+    <mergeCell ref="B4:G11"/>
+    <mergeCell ref="H4:L11"/>
+    <mergeCell ref="B13:L14"/>
+    <mergeCell ref="B15:G22"/>
+    <mergeCell ref="H15:L22"/>
+    <mergeCell ref="B50:L51"/>
+    <mergeCell ref="B52:G59"/>
+    <mergeCell ref="H52:L59"/>
+    <mergeCell ref="B61:L62"/>
+    <mergeCell ref="B63:G70"/>
+    <mergeCell ref="H63:L70"/>
+    <mergeCell ref="B26:L27"/>
+    <mergeCell ref="B28:G35"/>
+    <mergeCell ref="H28:L35"/>
+    <mergeCell ref="B37:L38"/>
+    <mergeCell ref="B39:G46"/>
+    <mergeCell ref="H39:L46"/>
+    <mergeCell ref="B98:L99"/>
+    <mergeCell ref="B100:G107"/>
+    <mergeCell ref="H100:L107"/>
+    <mergeCell ref="B109:L110"/>
+    <mergeCell ref="B111:G118"/>
+    <mergeCell ref="H111:L118"/>
+    <mergeCell ref="B74:L75"/>
+    <mergeCell ref="B76:G83"/>
+    <mergeCell ref="H76:L83"/>
+    <mergeCell ref="B85:L86"/>
+    <mergeCell ref="B87:G94"/>
+    <mergeCell ref="H87:L94"/>
+    <mergeCell ref="B146:L147"/>
+    <mergeCell ref="B148:G155"/>
+    <mergeCell ref="H148:L155"/>
+    <mergeCell ref="B157:L158"/>
+    <mergeCell ref="B159:G166"/>
+    <mergeCell ref="H159:L166"/>
+    <mergeCell ref="B122:L123"/>
+    <mergeCell ref="B124:G131"/>
+    <mergeCell ref="H124:L131"/>
+    <mergeCell ref="B133:L134"/>
+    <mergeCell ref="B135:G142"/>
+    <mergeCell ref="H135:L142"/>
+    <mergeCell ref="B194:L195"/>
+    <mergeCell ref="B196:G203"/>
+    <mergeCell ref="H196:L203"/>
+    <mergeCell ref="B205:L206"/>
+    <mergeCell ref="B207:G214"/>
+    <mergeCell ref="H207:L214"/>
+    <mergeCell ref="B170:L171"/>
+    <mergeCell ref="B172:G179"/>
+    <mergeCell ref="H172:L179"/>
+    <mergeCell ref="B181:L182"/>
+    <mergeCell ref="B183:G190"/>
+    <mergeCell ref="H183:L190"/>
+    <mergeCell ref="P26:Z27"/>
+    <mergeCell ref="P28:U35"/>
+    <mergeCell ref="V28:Z35"/>
+    <mergeCell ref="P37:Z38"/>
+    <mergeCell ref="P39:U46"/>
+    <mergeCell ref="V39:Z46"/>
+    <mergeCell ref="P2:Z3"/>
+    <mergeCell ref="P4:U11"/>
+    <mergeCell ref="V4:Z11"/>
+    <mergeCell ref="P13:Z14"/>
+    <mergeCell ref="P15:U22"/>
+    <mergeCell ref="V15:Z22"/>
+    <mergeCell ref="P74:Z75"/>
+    <mergeCell ref="P76:U83"/>
+    <mergeCell ref="V76:Z83"/>
+    <mergeCell ref="P85:Z86"/>
+    <mergeCell ref="P87:U94"/>
+    <mergeCell ref="V87:Z94"/>
+    <mergeCell ref="P50:Z51"/>
+    <mergeCell ref="P52:U59"/>
+    <mergeCell ref="V52:Z59"/>
+    <mergeCell ref="P61:Z62"/>
+    <mergeCell ref="P63:U70"/>
+    <mergeCell ref="V63:Z70"/>
+    <mergeCell ref="P122:Z123"/>
+    <mergeCell ref="P124:U131"/>
+    <mergeCell ref="V124:Z131"/>
+    <mergeCell ref="P133:Z134"/>
+    <mergeCell ref="P135:U142"/>
+    <mergeCell ref="V135:Z142"/>
+    <mergeCell ref="P98:Z99"/>
+    <mergeCell ref="P100:U107"/>
+    <mergeCell ref="V100:Z107"/>
+    <mergeCell ref="P109:Z110"/>
+    <mergeCell ref="P111:U118"/>
+    <mergeCell ref="V111:Z118"/>
+    <mergeCell ref="P170:Z171"/>
+    <mergeCell ref="P172:U179"/>
+    <mergeCell ref="V172:Z179"/>
+    <mergeCell ref="P181:Z182"/>
+    <mergeCell ref="P183:U190"/>
+    <mergeCell ref="V183:Z190"/>
+    <mergeCell ref="P146:Z147"/>
+    <mergeCell ref="P148:U155"/>
+    <mergeCell ref="V148:Z155"/>
+    <mergeCell ref="P157:Z158"/>
+    <mergeCell ref="P159:U166"/>
+    <mergeCell ref="V159:Z166"/>
+    <mergeCell ref="P218:Z219"/>
+    <mergeCell ref="P220:U227"/>
+    <mergeCell ref="V220:Z227"/>
+    <mergeCell ref="P229:Z230"/>
+    <mergeCell ref="P231:U238"/>
+    <mergeCell ref="V231:Z238"/>
+    <mergeCell ref="P194:Z195"/>
+    <mergeCell ref="P196:U203"/>
+    <mergeCell ref="V196:Z203"/>
+    <mergeCell ref="P205:Z206"/>
+    <mergeCell ref="P207:U214"/>
+    <mergeCell ref="V207:Z214"/>
+    <mergeCell ref="P266:Z267"/>
+    <mergeCell ref="P268:U275"/>
+    <mergeCell ref="V268:Z275"/>
+    <mergeCell ref="P277:Z278"/>
+    <mergeCell ref="P279:U286"/>
+    <mergeCell ref="V279:Z286"/>
+    <mergeCell ref="P242:Z243"/>
+    <mergeCell ref="P244:U251"/>
+    <mergeCell ref="V244:Z251"/>
+    <mergeCell ref="P253:Z254"/>
+    <mergeCell ref="P255:U262"/>
+    <mergeCell ref="V255:Z262"/>
+    <mergeCell ref="P314:Z315"/>
+    <mergeCell ref="P316:U323"/>
+    <mergeCell ref="V316:Z323"/>
+    <mergeCell ref="P325:Z326"/>
+    <mergeCell ref="P327:U334"/>
+    <mergeCell ref="V327:Z334"/>
+    <mergeCell ref="P290:Z291"/>
+    <mergeCell ref="P292:U299"/>
+    <mergeCell ref="V292:Z299"/>
+    <mergeCell ref="P301:Z302"/>
+    <mergeCell ref="P303:U310"/>
+    <mergeCell ref="V303:Z310"/>
     <mergeCell ref="P362:Z363"/>
     <mergeCell ref="P364:U371"/>
     <mergeCell ref="V364:Z371"/>
@@ -21211,144 +21430,6 @@
     <mergeCell ref="P349:Z350"/>
     <mergeCell ref="P351:U358"/>
     <mergeCell ref="V351:Z358"/>
-    <mergeCell ref="P314:Z315"/>
-    <mergeCell ref="P316:U323"/>
-    <mergeCell ref="V316:Z323"/>
-    <mergeCell ref="P325:Z326"/>
-    <mergeCell ref="P327:U334"/>
-    <mergeCell ref="V327:Z334"/>
-    <mergeCell ref="P290:Z291"/>
-    <mergeCell ref="P292:U299"/>
-    <mergeCell ref="V292:Z299"/>
-    <mergeCell ref="P301:Z302"/>
-    <mergeCell ref="P303:U310"/>
-    <mergeCell ref="V303:Z310"/>
-    <mergeCell ref="P266:Z267"/>
-    <mergeCell ref="P268:U275"/>
-    <mergeCell ref="V268:Z275"/>
-    <mergeCell ref="P277:Z278"/>
-    <mergeCell ref="P279:U286"/>
-    <mergeCell ref="V279:Z286"/>
-    <mergeCell ref="P242:Z243"/>
-    <mergeCell ref="P244:U251"/>
-    <mergeCell ref="V244:Z251"/>
-    <mergeCell ref="P253:Z254"/>
-    <mergeCell ref="P255:U262"/>
-    <mergeCell ref="V255:Z262"/>
-    <mergeCell ref="P218:Z219"/>
-    <mergeCell ref="P220:U227"/>
-    <mergeCell ref="V220:Z227"/>
-    <mergeCell ref="P229:Z230"/>
-    <mergeCell ref="P231:U238"/>
-    <mergeCell ref="V231:Z238"/>
-    <mergeCell ref="P194:Z195"/>
-    <mergeCell ref="P196:U203"/>
-    <mergeCell ref="V196:Z203"/>
-    <mergeCell ref="P205:Z206"/>
-    <mergeCell ref="P207:U214"/>
-    <mergeCell ref="V207:Z214"/>
-    <mergeCell ref="P170:Z171"/>
-    <mergeCell ref="P172:U179"/>
-    <mergeCell ref="V172:Z179"/>
-    <mergeCell ref="P181:Z182"/>
-    <mergeCell ref="P183:U190"/>
-    <mergeCell ref="V183:Z190"/>
-    <mergeCell ref="P146:Z147"/>
-    <mergeCell ref="P148:U155"/>
-    <mergeCell ref="V148:Z155"/>
-    <mergeCell ref="P157:Z158"/>
-    <mergeCell ref="P159:U166"/>
-    <mergeCell ref="V159:Z166"/>
-    <mergeCell ref="P122:Z123"/>
-    <mergeCell ref="P124:U131"/>
-    <mergeCell ref="V124:Z131"/>
-    <mergeCell ref="P133:Z134"/>
-    <mergeCell ref="P135:U142"/>
-    <mergeCell ref="V135:Z142"/>
-    <mergeCell ref="P98:Z99"/>
-    <mergeCell ref="P100:U107"/>
-    <mergeCell ref="V100:Z107"/>
-    <mergeCell ref="P109:Z110"/>
-    <mergeCell ref="P111:U118"/>
-    <mergeCell ref="V111:Z118"/>
-    <mergeCell ref="P74:Z75"/>
-    <mergeCell ref="P76:U83"/>
-    <mergeCell ref="V76:Z83"/>
-    <mergeCell ref="P85:Z86"/>
-    <mergeCell ref="P87:U94"/>
-    <mergeCell ref="V87:Z94"/>
-    <mergeCell ref="P50:Z51"/>
-    <mergeCell ref="P52:U59"/>
-    <mergeCell ref="V52:Z59"/>
-    <mergeCell ref="P61:Z62"/>
-    <mergeCell ref="P63:U70"/>
-    <mergeCell ref="V63:Z70"/>
-    <mergeCell ref="P26:Z27"/>
-    <mergeCell ref="P28:U35"/>
-    <mergeCell ref="V28:Z35"/>
-    <mergeCell ref="P37:Z38"/>
-    <mergeCell ref="P39:U46"/>
-    <mergeCell ref="V39:Z46"/>
-    <mergeCell ref="P2:Z3"/>
-    <mergeCell ref="P4:U11"/>
-    <mergeCell ref="V4:Z11"/>
-    <mergeCell ref="P13:Z14"/>
-    <mergeCell ref="P15:U22"/>
-    <mergeCell ref="V15:Z22"/>
-    <mergeCell ref="B194:L195"/>
-    <mergeCell ref="B196:G203"/>
-    <mergeCell ref="H196:L203"/>
-    <mergeCell ref="B205:L206"/>
-    <mergeCell ref="B207:G214"/>
-    <mergeCell ref="H207:L214"/>
-    <mergeCell ref="B170:L171"/>
-    <mergeCell ref="B172:G179"/>
-    <mergeCell ref="H172:L179"/>
-    <mergeCell ref="B181:L182"/>
-    <mergeCell ref="B183:G190"/>
-    <mergeCell ref="H183:L190"/>
-    <mergeCell ref="B146:L147"/>
-    <mergeCell ref="B148:G155"/>
-    <mergeCell ref="H148:L155"/>
-    <mergeCell ref="B157:L158"/>
-    <mergeCell ref="B159:G166"/>
-    <mergeCell ref="H159:L166"/>
-    <mergeCell ref="B122:L123"/>
-    <mergeCell ref="B124:G131"/>
-    <mergeCell ref="H124:L131"/>
-    <mergeCell ref="B133:L134"/>
-    <mergeCell ref="B135:G142"/>
-    <mergeCell ref="H135:L142"/>
-    <mergeCell ref="B98:L99"/>
-    <mergeCell ref="B100:G107"/>
-    <mergeCell ref="H100:L107"/>
-    <mergeCell ref="B109:L110"/>
-    <mergeCell ref="B111:G118"/>
-    <mergeCell ref="H111:L118"/>
-    <mergeCell ref="B74:L75"/>
-    <mergeCell ref="B76:G83"/>
-    <mergeCell ref="H76:L83"/>
-    <mergeCell ref="B85:L86"/>
-    <mergeCell ref="B87:G94"/>
-    <mergeCell ref="H87:L94"/>
-    <mergeCell ref="B50:L51"/>
-    <mergeCell ref="B52:G59"/>
-    <mergeCell ref="H52:L59"/>
-    <mergeCell ref="B61:L62"/>
-    <mergeCell ref="B63:G70"/>
-    <mergeCell ref="H63:L70"/>
-    <mergeCell ref="B26:L27"/>
-    <mergeCell ref="B28:G35"/>
-    <mergeCell ref="H28:L35"/>
-    <mergeCell ref="B37:L38"/>
-    <mergeCell ref="B39:G46"/>
-    <mergeCell ref="H39:L46"/>
-    <mergeCell ref="B2:L3"/>
-    <mergeCell ref="B4:G11"/>
-    <mergeCell ref="H4:L11"/>
-    <mergeCell ref="B13:L14"/>
-    <mergeCell ref="B15:G22"/>
-    <mergeCell ref="H15:L22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -21800,7 +21881,7 @@
         <v>396</v>
       </c>
       <c r="E16" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="F16" t="s">
         <v>23</v>
@@ -21808,7 +21889,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -21830,7 +21911,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="B18">
         <v>2</v>
@@ -21852,7 +21933,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="B19">
         <v>3</v>
@@ -21874,7 +21955,7 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B20">
         <v>5</v>
@@ -21896,7 +21977,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B21">
         <v>6</v>
@@ -21918,7 +21999,7 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="B22">
         <v>8</v>
@@ -21940,7 +22021,7 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="B23">
         <v>9</v>
@@ -21962,7 +22043,7 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="B24">
         <v>10</v>
@@ -22289,7 +22370,7 @@
         <v>488</v>
       </c>
       <c r="B41" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="C41" t="s">
         <v>23</v>
@@ -22303,7 +22384,7 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="B42">
         <v>0</v>
@@ -22312,7 +22393,7 @@
         <v>0</v>
       </c>
       <c r="F42" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="G42">
         <v>10</v>
@@ -22320,7 +22401,7 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="B43">
         <v>3</v>
@@ -22331,7 +22412,7 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="B44">
         <v>6</v>
@@ -22346,12 +22427,12 @@
         <v>73</v>
       </c>
       <c r="H44" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B45">
         <v>11</v>
@@ -22371,7 +22452,7 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B46">
         <v>14</v>
@@ -22382,7 +22463,7 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="B47">
         <v>16</v>
@@ -22393,7 +22474,7 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="B48">
         <v>20</v>
@@ -22404,7 +22485,7 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="B49">
         <v>21</v>
@@ -22415,7 +22496,7 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="B50">
         <v>21</v>
@@ -22426,7 +22507,7 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="B51">
         <v>28</v>
@@ -22437,7 +22518,7 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="B52">
         <v>33</v>
@@ -22448,7 +22529,7 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="B53">
         <v>40</v>
@@ -22459,7 +22540,7 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="B54">
         <v>49</v>
@@ -22470,7 +22551,7 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="B55">
         <v>55</v>
@@ -22481,7 +22562,7 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="B56">
         <v>60</v>
@@ -22492,7 +22573,7 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="B57">
         <v>65</v>
@@ -22503,7 +22584,7 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="B58">
         <v>71</v>
@@ -22514,7 +22595,7 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="B59">
         <v>79</v>
@@ -22525,7 +22606,7 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="B60">
         <v>86</v>
@@ -22536,7 +22617,7 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="B61">
         <v>91</v>

</xml_diff>